<commit_message>
18 / 09 / 2024
</commit_message>
<xml_diff>
--- a/Data/reliance.xlsx
+++ b/Data/reliance.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1165"/>
+  <dimension ref="A1:G1169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
         <v>1380.276611328125</v>
       </c>
       <c r="F2" t="n">
-        <v>1356.042846679688</v>
+        <v>1356.042724609375</v>
       </c>
       <c r="G2" t="n">
         <v>7002234</v>
@@ -562,7 +562,7 @@
         <v>1372.87060546875</v>
       </c>
       <c r="F5" t="n">
-        <v>1348.766723632812</v>
+        <v>1348.766845703125</v>
       </c>
       <c r="G5" t="n">
         <v>12259588</v>
@@ -608,7 +608,7 @@
         <v>1383.522583007812</v>
       </c>
       <c r="F7" t="n">
-        <v>1359.231689453125</v>
+        <v>1359.231811523438</v>
       </c>
       <c r="G7" t="n">
         <v>8023951</v>
@@ -631,7 +631,7 @@
         <v>1415.387084960938</v>
       </c>
       <c r="F8" t="n">
-        <v>1390.536743164062</v>
+        <v>1390.536865234375</v>
       </c>
       <c r="G8" t="n">
         <v>7491371</v>
@@ -700,7 +700,7 @@
         <v>1398.380493164062</v>
       </c>
       <c r="F11" t="n">
-        <v>1373.828979492188</v>
+        <v>1373.828735351562</v>
       </c>
       <c r="G11" t="n">
         <v>7908267</v>
@@ -723,7 +723,7 @@
         <v>1393.305908203125</v>
       </c>
       <c r="F12" t="n">
-        <v>1368.84326171875</v>
+        <v>1368.843383789062</v>
       </c>
       <c r="G12" t="n">
         <v>7908929</v>
@@ -769,7 +769,7 @@
         <v>1445.56005859375</v>
       </c>
       <c r="F14" t="n">
-        <v>1420.179931640625</v>
+        <v>1420.179809570312</v>
       </c>
       <c r="G14" t="n">
         <v>14731735</v>
@@ -815,7 +815,7 @@
         <v>1402.494995117188</v>
       </c>
       <c r="F16" t="n">
-        <v>1377.87109375</v>
+        <v>1377.871215820312</v>
       </c>
       <c r="G16" t="n">
         <v>9461360</v>
@@ -838,7 +838,7 @@
         <v>1401.992065429688</v>
       </c>
       <c r="F17" t="n">
-        <v>1377.377075195312</v>
+        <v>1377.376953125</v>
       </c>
       <c r="G17" t="n">
         <v>5161408</v>
@@ -861,7 +861,7 @@
         <v>1396.048950195312</v>
       </c>
       <c r="F18" t="n">
-        <v>1371.538208007812</v>
+        <v>1371.538330078125</v>
       </c>
       <c r="G18" t="n">
         <v>5623869</v>
@@ -884,7 +884,7 @@
         <v>1391.203002929688</v>
       </c>
       <c r="F19" t="n">
-        <v>1366.77734375</v>
+        <v>1366.777221679688</v>
       </c>
       <c r="G19" t="n">
         <v>7314222</v>
@@ -930,7 +930,7 @@
         <v>1345.669189453125</v>
       </c>
       <c r="F21" t="n">
-        <v>1322.042846679688</v>
+        <v>1322.04296875</v>
       </c>
       <c r="G21" t="n">
         <v>12266118</v>
@@ -999,7 +999,7 @@
         <v>1290.7177734375</v>
       </c>
       <c r="F24" t="n">
-        <v>1268.056518554688</v>
+        <v>1268.056396484375</v>
       </c>
       <c r="G24" t="n">
         <v>17375155</v>
@@ -1091,7 +1091,7 @@
         <v>1332.914184570312</v>
       </c>
       <c r="F28" t="n">
-        <v>1309.511962890625</v>
+        <v>1309.511840820312</v>
       </c>
       <c r="G28" t="n">
         <v>7769288</v>
@@ -1160,7 +1160,7 @@
         <v>1328.296875</v>
       </c>
       <c r="F31" t="n">
-        <v>1304.975708007812</v>
+        <v>1304.9755859375</v>
       </c>
       <c r="G31" t="n">
         <v>6999908</v>
@@ -1252,7 +1252,7 @@
         <v>1351.6123046875</v>
       </c>
       <c r="F35" t="n">
-        <v>1327.8818359375</v>
+        <v>1327.881713867188</v>
       </c>
       <c r="G35" t="n">
         <v>6574565</v>
@@ -1275,7 +1275,7 @@
         <v>1341.691772460938</v>
       </c>
       <c r="F36" t="n">
-        <v>1318.13525390625</v>
+        <v>1318.135498046875</v>
       </c>
       <c r="G36" t="n">
         <v>5563580</v>
@@ -1367,7 +1367,7 @@
         <v>1295.060913085938</v>
       </c>
       <c r="F40" t="n">
-        <v>1272.3232421875</v>
+        <v>1272.323120117188</v>
       </c>
       <c r="G40" t="n">
         <v>13872531</v>
@@ -1482,7 +1482,7 @@
         <v>1227.811645507812</v>
       </c>
       <c r="F45" t="n">
-        <v>1206.254760742188</v>
+        <v>1206.254638671875</v>
       </c>
       <c r="G45" t="n">
         <v>13699399</v>
@@ -1528,7 +1528,7 @@
         <v>1198.827392578125</v>
       </c>
       <c r="F47" t="n">
-        <v>1177.779174804688</v>
+        <v>1177.779296875</v>
       </c>
       <c r="G47" t="n">
         <v>15255195</v>
@@ -1551,7 +1551,7 @@
         <v>1162.116821289062</v>
       </c>
       <c r="F48" t="n">
-        <v>1141.713256835938</v>
+        <v>1141.71337890625</v>
       </c>
       <c r="G48" t="n">
         <v>16867019</v>
@@ -1574,7 +1574,7 @@
         <v>1018.703796386719</v>
       </c>
       <c r="F49" t="n">
-        <v>1000.818237304688</v>
+        <v>1000.818176269531</v>
       </c>
       <c r="G49" t="n">
         <v>44093509</v>
@@ -1597,7 +1597,7 @@
         <v>1054.728515625</v>
       </c>
       <c r="F50" t="n">
-        <v>1036.210327148438</v>
+        <v>1036.21044921875</v>
       </c>
       <c r="G50" t="n">
         <v>29789288</v>
@@ -1689,7 +1689,7 @@
         <v>921.6473999023438</v>
       </c>
       <c r="F54" t="n">
-        <v>905.4657592773438</v>
+        <v>905.4658203125</v>
       </c>
       <c r="G54" t="n">
         <v>22722989</v>
@@ -1735,7 +1735,7 @@
         <v>839.0831298828125</v>
       </c>
       <c r="F56" t="n">
-        <v>824.3511352539062</v>
+        <v>824.35107421875</v>
       </c>
       <c r="G56" t="n">
         <v>30702005</v>
@@ -1781,7 +1781,7 @@
         <v>808.3158569335938</v>
       </c>
       <c r="F58" t="n">
-        <v>794.1240844726562</v>
+        <v>794.1241455078125</v>
       </c>
       <c r="G58" t="n">
         <v>20335474</v>
@@ -1804,7 +1804,7 @@
         <v>862.5814819335938</v>
       </c>
       <c r="F59" t="n">
-        <v>847.4368896484375</v>
+        <v>847.4369506835938</v>
       </c>
       <c r="G59" t="n">
         <v>22867443</v>
@@ -1827,7 +1827,7 @@
         <v>989.5365600585938</v>
       </c>
       <c r="F60" t="n">
-        <v>972.1630859375</v>
+        <v>972.1630249023438</v>
       </c>
       <c r="G60" t="n">
         <v>36565149</v>
@@ -1850,7 +1850,7 @@
         <v>974.8615112304688</v>
       </c>
       <c r="F61" t="n">
-        <v>957.74560546875</v>
+        <v>957.7456665039062</v>
       </c>
       <c r="G61" t="n">
         <v>22872244</v>
@@ -1873,7 +1873,7 @@
         <v>974.3129272460938</v>
       </c>
       <c r="F62" t="n">
-        <v>957.206787109375</v>
+        <v>957.2066650390625</v>
       </c>
       <c r="G62" t="n">
         <v>20828970</v>
@@ -1919,7 +1919,7 @@
         <v>1018.338073730469</v>
       </c>
       <c r="F64" t="n">
-        <v>1000.458862304688</v>
+        <v>1000.458923339844</v>
       </c>
       <c r="G64" t="n">
         <v>22146405</v>
@@ -1942,7 +1942,7 @@
         <v>987.8908081054688</v>
       </c>
       <c r="F65" t="n">
-        <v>970.546142578125</v>
+        <v>970.5460815429688</v>
       </c>
       <c r="G65" t="n">
         <v>20798729</v>
@@ -1988,7 +1988,7 @@
         <v>1102.776733398438</v>
       </c>
       <c r="F67" t="n">
-        <v>1083.415161132812</v>
+        <v>1083.4150390625</v>
       </c>
       <c r="G67" t="n">
         <v>27186812</v>
@@ -2011,7 +2011,7 @@
         <v>1090.021728515625</v>
       </c>
       <c r="F68" t="n">
-        <v>1070.884033203125</v>
+        <v>1070.883911132812</v>
       </c>
       <c r="G68" t="n">
         <v>24940165</v>
@@ -2057,7 +2057,7 @@
         <v>1087.27880859375</v>
       </c>
       <c r="F70" t="n">
-        <v>1068.189208984375</v>
+        <v>1068.189331054688</v>
       </c>
       <c r="G70" t="n">
         <v>11836892</v>
@@ -2103,7 +2103,7 @@
         <v>1067.986328125</v>
       </c>
       <c r="F72" t="n">
-        <v>1049.2353515625</v>
+        <v>1049.235229492188</v>
       </c>
       <c r="G72" t="n">
         <v>18727853</v>
@@ -2149,7 +2149,7 @@
         <v>1137.2470703125</v>
       </c>
       <c r="F74" t="n">
-        <v>1117.280029296875</v>
+        <v>1117.280151367188</v>
       </c>
       <c r="G74" t="n">
         <v>18015466</v>
@@ -2172,7 +2172,7 @@
         <v>1131.349609375</v>
       </c>
       <c r="F75" t="n">
-        <v>1111.486206054688</v>
+        <v>1111.486328125</v>
       </c>
       <c r="G75" t="n">
         <v>30685814</v>
@@ -2218,7 +2218,7 @@
         <v>1253.458740234375</v>
       </c>
       <c r="F77" t="n">
-        <v>1231.451416015625</v>
+        <v>1231.451538085938</v>
       </c>
       <c r="G77" t="n">
         <v>32732251</v>
@@ -2241,7 +2241,7 @@
         <v>1295.609497070312</v>
       </c>
       <c r="F78" t="n">
-        <v>1272.862182617188</v>
+        <v>1272.8623046875</v>
       </c>
       <c r="G78" t="n">
         <v>67493154</v>
@@ -2264,7 +2264,7 @@
         <v>1307.267211914062</v>
       </c>
       <c r="F79" t="n">
-        <v>1284.315307617188</v>
+        <v>1284.315185546875</v>
       </c>
       <c r="G79" t="n">
         <v>29241450</v>
@@ -2287,7 +2287,7 @@
         <v>1305.804321289062</v>
       </c>
       <c r="F80" t="n">
-        <v>1282.878051757812</v>
+        <v>1282.878173828125</v>
       </c>
       <c r="G80" t="n">
         <v>39226700</v>
@@ -2333,7 +2333,7 @@
         <v>1340.411743164062</v>
       </c>
       <c r="F82" t="n">
-        <v>1316.877807617188</v>
+        <v>1316.8779296875</v>
       </c>
       <c r="G82" t="n">
         <v>35672949</v>
@@ -2379,7 +2379,7 @@
         <v>1335.52001953125</v>
       </c>
       <c r="F84" t="n">
-        <v>1312.071899414062</v>
+        <v>1312.072021484375</v>
       </c>
       <c r="G84" t="n">
         <v>22451881</v>
@@ -2425,7 +2425,7 @@
         <v>1377.853637695312</v>
       </c>
       <c r="F86" t="n">
-        <v>1353.662353515625</v>
+        <v>1353.662231445312</v>
       </c>
       <c r="G86" t="n">
         <v>25013483</v>
@@ -2517,7 +2517,7 @@
         <v>1381.222900390625</v>
       </c>
       <c r="F90" t="n">
-        <v>1356.972412109375</v>
+        <v>1356.972534179688</v>
       </c>
       <c r="G90" t="n">
         <v>33215062</v>
@@ -2540,7 +2540,7 @@
         <v>1325.38134765625</v>
       </c>
       <c r="F91" t="n">
-        <v>1302.111206054688</v>
+        <v>1302.111328125</v>
       </c>
       <c r="G91" t="n">
         <v>24633385</v>
@@ -2563,7 +2563,7 @@
         <v>1347.025756835938</v>
       </c>
       <c r="F92" t="n">
-        <v>1323.375854492188</v>
+        <v>1323.375732421875</v>
       </c>
       <c r="G92" t="n">
         <v>31076130</v>
@@ -2701,7 +2701,7 @@
         <v>1314.397705078125</v>
       </c>
       <c r="F98" t="n">
-        <v>1291.320556640625</v>
+        <v>1291.320434570312</v>
       </c>
       <c r="G98" t="n">
         <v>16608317</v>
@@ -2747,7 +2747,7 @@
         <v>1358.88623046875</v>
       </c>
       <c r="F100" t="n">
-        <v>1335.027954101562</v>
+        <v>1335.02783203125</v>
       </c>
       <c r="G100" t="n">
         <v>20063139</v>
@@ -2770,7 +2770,7 @@
         <v>1351.640747070312</v>
       </c>
       <c r="F101" t="n">
-        <v>1327.90966796875</v>
+        <v>1327.909545898438</v>
       </c>
       <c r="G101" t="n">
         <v>20011263</v>
@@ -2816,7 +2816,7 @@
         <v>1417.450561523438</v>
       </c>
       <c r="F103" t="n">
-        <v>1392.564086914062</v>
+        <v>1392.56396484375</v>
       </c>
       <c r="G103" t="n">
         <v>11076980</v>
@@ -2862,7 +2862,7 @@
         <v>1458.154907226562</v>
       </c>
       <c r="F105" t="n">
-        <v>1432.5537109375</v>
+        <v>1432.553833007812</v>
       </c>
       <c r="G105" t="n">
         <v>17101175</v>
@@ -2954,7 +2954,7 @@
         <v>1451.093994140625</v>
       </c>
       <c r="F109" t="n">
-        <v>1425.61669921875</v>
+        <v>1425.616821289062</v>
       </c>
       <c r="G109" t="n">
         <v>11066323</v>
@@ -3000,7 +3000,7 @@
         <v>1466.4619140625</v>
       </c>
       <c r="F111" t="n">
-        <v>1440.71484375</v>
+        <v>1440.714965820312</v>
       </c>
       <c r="G111" t="n">
         <v>19274449</v>
@@ -3023,7 +3023,7 @@
         <v>1490.229125976562</v>
       </c>
       <c r="F112" t="n">
-        <v>1464.06494140625</v>
+        <v>1464.064819335938</v>
       </c>
       <c r="G112" t="n">
         <v>26553701</v>
@@ -3161,7 +3161,7 @@
         <v>1588.39013671875</v>
       </c>
       <c r="F118" t="n">
-        <v>1560.502563476562</v>
+        <v>1560.502319335938</v>
       </c>
       <c r="G118" t="n">
         <v>18981039</v>
@@ -3184,7 +3184,7 @@
         <v>1594.804931640625</v>
       </c>
       <c r="F119" t="n">
-        <v>1566.804809570312</v>
+        <v>1566.804565429688</v>
       </c>
       <c r="G119" t="n">
         <v>25793110</v>
@@ -3276,7 +3276,7 @@
         <v>1572.8837890625</v>
       </c>
       <c r="F123" t="n">
-        <v>1545.268310546875</v>
+        <v>1545.268432617188</v>
       </c>
       <c r="G123" t="n">
         <v>15138210</v>
@@ -3483,7 +3483,7 @@
         <v>1786.00439453125</v>
       </c>
       <c r="F132" t="n">
-        <v>1761.787475585938</v>
+        <v>1761.787353515625</v>
       </c>
       <c r="G132" t="n">
         <v>34804196</v>
@@ -3506,7 +3506,7 @@
         <v>1769.390380859375</v>
       </c>
       <c r="F133" t="n">
-        <v>1745.398681640625</v>
+        <v>1745.398559570312</v>
       </c>
       <c r="G133" t="n">
         <v>33665564</v>
@@ -3529,7 +3529,7 @@
         <v>1702.011352539062</v>
       </c>
       <c r="F134" t="n">
-        <v>1678.933227539062</v>
+        <v>1678.933349609375</v>
       </c>
       <c r="G134" t="n">
         <v>69834886</v>
@@ -3575,7 +3575,7 @@
         <v>1764.49853515625</v>
       </c>
       <c r="F136" t="n">
-        <v>1740.5732421875</v>
+        <v>1740.573120117188</v>
       </c>
       <c r="G136" t="n">
         <v>24863382</v>
@@ -3667,7 +3667,7 @@
         <v>1899.348754882812</v>
       </c>
       <c r="F140" t="n">
-        <v>1873.594848632812</v>
+        <v>1873.594970703125</v>
       </c>
       <c r="G140" t="n">
         <v>29166875</v>
@@ -3690,7 +3690,7 @@
         <v>1980.895751953125</v>
       </c>
       <c r="F141" t="n">
-        <v>1954.036010742188</v>
+        <v>1954.0361328125</v>
       </c>
       <c r="G141" t="n">
         <v>60298686</v>
@@ -3782,7 +3782,7 @@
         <v>1946.467895507812</v>
       </c>
       <c r="F145" t="n">
-        <v>1920.075073242188</v>
+        <v>1920.0751953125</v>
       </c>
       <c r="G145" t="n">
         <v>36428722</v>
@@ -3828,7 +3828,7 @@
         <v>1854.306396484375</v>
       </c>
       <c r="F147" t="n">
-        <v>1829.163208007812</v>
+        <v>1829.163330078125</v>
       </c>
       <c r="G147" t="n">
         <v>23357691</v>
@@ -3897,7 +3897,7 @@
         <v>1969.773559570312</v>
       </c>
       <c r="F150" t="n">
-        <v>1943.06494140625</v>
+        <v>1943.064819335938</v>
       </c>
       <c r="G150" t="n">
         <v>24661487</v>
@@ -3920,7 +3920,7 @@
         <v>1981.172607421875</v>
       </c>
       <c r="F151" t="n">
-        <v>1954.309326171875</v>
+        <v>1954.309204101562</v>
       </c>
       <c r="G151" t="n">
         <v>16492208</v>
@@ -3943,7 +3943,7 @@
         <v>1956.620849609375</v>
       </c>
       <c r="F152" t="n">
-        <v>1930.09033203125</v>
+        <v>1930.090454101562</v>
       </c>
       <c r="G152" t="n">
         <v>13479498</v>
@@ -4035,7 +4035,7 @@
         <v>1951.036743164062</v>
       </c>
       <c r="F156" t="n">
-        <v>1924.58203125</v>
+        <v>1924.582153320312</v>
       </c>
       <c r="G156" t="n">
         <v>16612317</v>
@@ -4058,7 +4058,7 @@
         <v>1930.3154296875</v>
       </c>
       <c r="F157" t="n">
-        <v>1904.1416015625</v>
+        <v>1904.141723632812</v>
       </c>
       <c r="G157" t="n">
         <v>15489533</v>
@@ -4081,7 +4081,7 @@
         <v>1955.421020507812</v>
       </c>
       <c r="F158" t="n">
-        <v>1928.906860351562</v>
+        <v>1928.906982421875</v>
       </c>
       <c r="G158" t="n">
         <v>15273836</v>
@@ -4127,7 +4127,7 @@
         <v>1935.576416015625</v>
       </c>
       <c r="F160" t="n">
-        <v>1909.331298828125</v>
+        <v>1909.331420898438</v>
       </c>
       <c r="G160" t="n">
         <v>11268922</v>
@@ -4173,7 +4173,7 @@
         <v>1934.376586914062</v>
       </c>
       <c r="F162" t="n">
-        <v>1908.147583007812</v>
+        <v>1908.147827148438</v>
       </c>
       <c r="G162" t="n">
         <v>16358609</v>
@@ -4196,7 +4196,7 @@
         <v>1921.777587890625</v>
       </c>
       <c r="F163" t="n">
-        <v>1895.7197265625</v>
+        <v>1895.719604492188</v>
       </c>
       <c r="G163" t="n">
         <v>9694004</v>
@@ -4242,7 +4242,7 @@
         <v>1948.083129882812</v>
       </c>
       <c r="F165" t="n">
-        <v>1921.66845703125</v>
+        <v>1921.668579101562</v>
       </c>
       <c r="G165" t="n">
         <v>14042531</v>
@@ -4265,7 +4265,7 @@
         <v>1953.205810546875</v>
       </c>
       <c r="F166" t="n">
-        <v>1926.7216796875</v>
+        <v>1926.721801757812</v>
       </c>
       <c r="G166" t="n">
         <v>13583450</v>
@@ -4334,7 +4334,7 @@
         <v>1964.327880859375</v>
       </c>
       <c r="F169" t="n">
-        <v>1937.692993164062</v>
+        <v>1937.69287109375</v>
       </c>
       <c r="G169" t="n">
         <v>13474719</v>
@@ -4357,7 +4357,7 @@
         <v>1949.467651367188</v>
       </c>
       <c r="F170" t="n">
-        <v>1923.034301757812</v>
+        <v>1923.0341796875</v>
       </c>
       <c r="G170" t="n">
         <v>9293214</v>
@@ -4380,7 +4380,7 @@
         <v>1917.301025390625</v>
       </c>
       <c r="F171" t="n">
-        <v>1891.303833007812</v>
+        <v>1891.3037109375</v>
       </c>
       <c r="G171" t="n">
         <v>14237972</v>
@@ -4403,7 +4403,7 @@
         <v>1922.285278320312</v>
       </c>
       <c r="F172" t="n">
-        <v>1896.220336914062</v>
+        <v>1896.220581054688</v>
       </c>
       <c r="G172" t="n">
         <v>10963236</v>
@@ -4426,7 +4426,7 @@
         <v>1944.852661132812</v>
       </c>
       <c r="F173" t="n">
-        <v>1918.481689453125</v>
+        <v>1918.481811523438</v>
       </c>
       <c r="G173" t="n">
         <v>13698541</v>
@@ -4610,7 +4610,7 @@
         <v>2128.160400390625</v>
       </c>
       <c r="F181" t="n">
-        <v>2099.303955078125</v>
+        <v>2099.3037109375</v>
       </c>
       <c r="G181" t="n">
         <v>16537457</v>
@@ -4633,7 +4633,7 @@
         <v>2082.14892578125</v>
       </c>
       <c r="F182" t="n">
-        <v>2053.916259765625</v>
+        <v>2053.91650390625</v>
       </c>
       <c r="G182" t="n">
         <v>16813690</v>
@@ -4679,7 +4679,7 @@
         <v>2059.027587890625</v>
       </c>
       <c r="F184" t="n">
-        <v>2031.108642578125</v>
+        <v>2031.108520507812</v>
       </c>
       <c r="G184" t="n">
         <v>21494354</v>
@@ -4702,7 +4702,7 @@
         <v>2013.246948242188</v>
       </c>
       <c r="F185" t="n">
-        <v>1985.94873046875</v>
+        <v>1985.948852539062</v>
       </c>
       <c r="G185" t="n">
         <v>14913159</v>
@@ -4748,7 +4748,7 @@
         <v>2045.598022460938</v>
       </c>
       <c r="F187" t="n">
-        <v>2017.861206054688</v>
+        <v>2017.861083984375</v>
       </c>
       <c r="G187" t="n">
         <v>9833424</v>
@@ -4771,7 +4771,7 @@
         <v>2072.180419921875</v>
       </c>
       <c r="F188" t="n">
-        <v>2044.082885742188</v>
+        <v>2044.083129882812</v>
       </c>
       <c r="G188" t="n">
         <v>12921269</v>
@@ -4794,7 +4794,7 @@
         <v>2062.304443359375</v>
       </c>
       <c r="F189" t="n">
-        <v>2034.340942382812</v>
+        <v>2034.341064453125</v>
       </c>
       <c r="G189" t="n">
         <v>12232579</v>
@@ -4817,7 +4817,7 @@
         <v>2053.905029296875</v>
       </c>
       <c r="F190" t="n">
-        <v>2026.055419921875</v>
+        <v>2026.055541992188</v>
       </c>
       <c r="G190" t="n">
         <v>10391613</v>
@@ -4909,7 +4909,7 @@
         <v>2066.826904296875</v>
       </c>
       <c r="F194" t="n">
-        <v>2038.80224609375</v>
+        <v>2038.802124023438</v>
       </c>
       <c r="G194" t="n">
         <v>10538904</v>
@@ -4932,7 +4932,7 @@
         <v>2061.4736328125</v>
       </c>
       <c r="F195" t="n">
-        <v>2033.521484375</v>
+        <v>2033.521362304688</v>
       </c>
       <c r="G195" t="n">
         <v>9272749</v>
@@ -4955,7 +4955,7 @@
         <v>2064.79638671875</v>
       </c>
       <c r="F196" t="n">
-        <v>2036.799194335938</v>
+        <v>2036.799072265625</v>
       </c>
       <c r="G196" t="n">
         <v>7113236</v>
@@ -4978,7 +4978,7 @@
         <v>2105.08544921875</v>
       </c>
       <c r="F197" t="n">
-        <v>2076.5419921875</v>
+        <v>2076.542236328125</v>
       </c>
       <c r="G197" t="n">
         <v>11556006</v>
@@ -5024,7 +5024,7 @@
         <v>2036.598754882812</v>
       </c>
       <c r="F199" t="n">
-        <v>2008.983764648438</v>
+        <v>2008.98388671875</v>
       </c>
       <c r="G199" t="n">
         <v>10018098</v>
@@ -5070,7 +5070,7 @@
         <v>2008.6318359375</v>
       </c>
       <c r="F201" t="n">
-        <v>1981.396240234375</v>
+        <v>1981.396118164062</v>
       </c>
       <c r="G201" t="n">
         <v>15600192</v>
@@ -5208,7 +5208,7 @@
         <v>1877.842895507812</v>
       </c>
       <c r="F207" t="n">
-        <v>1852.380615234375</v>
+        <v>1852.380737304688</v>
       </c>
       <c r="G207" t="n">
         <v>18239448</v>
@@ -5231,7 +5231,7 @@
         <v>1856.567749023438</v>
       </c>
       <c r="F208" t="n">
-        <v>1831.393798828125</v>
+        <v>1831.39404296875</v>
       </c>
       <c r="G208" t="n">
         <v>14962008</v>
@@ -5277,7 +5277,7 @@
         <v>1896.302856445312</v>
       </c>
       <c r="F210" t="n">
-        <v>1870.590209960938</v>
+        <v>1870.59033203125</v>
       </c>
       <c r="G210" t="n">
         <v>17010781</v>
@@ -5323,7 +5323,7 @@
         <v>1707.918579101562</v>
       </c>
       <c r="F212" t="n">
-        <v>1684.760375976562</v>
+        <v>1684.760498046875</v>
       </c>
       <c r="G212" t="n">
         <v>44345811</v>
@@ -5346,7 +5346,7 @@
         <v>1765.882934570312</v>
       </c>
       <c r="F213" t="n">
-        <v>1741.938720703125</v>
+        <v>1741.938842773438</v>
       </c>
       <c r="G213" t="n">
         <v>40090058</v>
@@ -5461,7 +5461,7 @@
         <v>1843.414916992188</v>
       </c>
       <c r="F218" t="n">
-        <v>1818.419555664062</v>
+        <v>1818.419311523438</v>
       </c>
       <c r="G218" t="n">
         <v>28362390</v>
@@ -5530,7 +5530,7 @@
         <v>1848.122192382812</v>
       </c>
       <c r="F221" t="n">
-        <v>1823.063110351562</v>
+        <v>1823.062866210938</v>
       </c>
       <c r="G221" t="n">
         <v>2613110</v>
@@ -5599,7 +5599,7 @@
         <v>1821.216796875</v>
       </c>
       <c r="F224" t="n">
-        <v>1796.5224609375</v>
+        <v>1796.522338867188</v>
       </c>
       <c r="G224" t="n">
         <v>13898171</v>
@@ -5645,7 +5645,7 @@
         <v>1800.495483398438</v>
       </c>
       <c r="F226" t="n">
-        <v>1776.081909179688</v>
+        <v>1776.08203125</v>
       </c>
       <c r="G226" t="n">
         <v>22663783</v>
@@ -5714,7 +5714,7 @@
         <v>1802.249145507812</v>
       </c>
       <c r="F229" t="n">
-        <v>1777.81201171875</v>
+        <v>1777.811889648438</v>
       </c>
       <c r="G229" t="n">
         <v>12919318</v>
@@ -5783,7 +5783,7 @@
         <v>1807.371826171875</v>
       </c>
       <c r="F232" t="n">
-        <v>1782.865234375</v>
+        <v>1782.865112304688</v>
       </c>
       <c r="G232" t="n">
         <v>11094443</v>
@@ -5829,7 +5829,7 @@
         <v>1796.849609375</v>
       </c>
       <c r="F234" t="n">
-        <v>1772.485473632812</v>
+        <v>1772.485595703125</v>
       </c>
       <c r="G234" t="n">
         <v>9232276</v>
@@ -5875,7 +5875,7 @@
         <v>1840.230590820312</v>
       </c>
       <c r="F236" t="n">
-        <v>1815.2783203125</v>
+        <v>1815.278198242188</v>
       </c>
       <c r="G236" t="n">
         <v>21701530</v>
@@ -5898,7 +5898,7 @@
         <v>1870.874145507812</v>
       </c>
       <c r="F237" t="n">
-        <v>1845.506469726562</v>
+        <v>1845.50634765625</v>
       </c>
       <c r="G237" t="n">
         <v>14587627</v>
@@ -5921,7 +5921,7 @@
         <v>1852.460327148438</v>
       </c>
       <c r="F238" t="n">
-        <v>1827.342163085938</v>
+        <v>1827.34228515625</v>
       </c>
       <c r="G238" t="n">
         <v>8032753</v>
@@ -6036,7 +6036,7 @@
         <v>1832.708129882812</v>
       </c>
       <c r="F243" t="n">
-        <v>1807.858032226562</v>
+        <v>1807.85791015625</v>
       </c>
       <c r="G243" t="n">
         <v>10126179</v>
@@ -6059,7 +6059,7 @@
         <v>1838.199951171875</v>
       </c>
       <c r="F244" t="n">
-        <v>1813.275146484375</v>
+        <v>1813.275268554688</v>
       </c>
       <c r="G244" t="n">
         <v>9233172</v>
@@ -6151,7 +6151,7 @@
         <v>1840.599853515625</v>
       </c>
       <c r="F248" t="n">
-        <v>1815.642578125</v>
+        <v>1815.642700195312</v>
       </c>
       <c r="G248" t="n">
         <v>10388494</v>
@@ -6197,7 +6197,7 @@
         <v>1836.815551757812</v>
       </c>
       <c r="F250" t="n">
-        <v>1811.90966796875</v>
+        <v>1811.909545898438</v>
       </c>
       <c r="G250" t="n">
         <v>9305969</v>
@@ -6220,7 +6220,7 @@
         <v>1841.845825195312</v>
       </c>
       <c r="F251" t="n">
-        <v>1816.87158203125</v>
+        <v>1816.871704101562</v>
       </c>
       <c r="G251" t="n">
         <v>11021815</v>
@@ -6243,7 +6243,7 @@
         <v>1832.431274414062</v>
       </c>
       <c r="F252" t="n">
-        <v>1807.584716796875</v>
+        <v>1807.584838867188</v>
       </c>
       <c r="G252" t="n">
         <v>9390594</v>
@@ -6312,7 +6312,7 @@
         <v>1814.709716796875</v>
       </c>
       <c r="F255" t="n">
-        <v>1790.103515625</v>
+        <v>1790.103393554688</v>
       </c>
       <c r="G255" t="n">
         <v>12061545</v>
@@ -6335,7 +6335,7 @@
         <v>1766.852172851562</v>
       </c>
       <c r="F256" t="n">
-        <v>1742.894775390625</v>
+        <v>1742.894897460938</v>
       </c>
       <c r="G256" t="n">
         <v>23200734</v>
@@ -6358,7 +6358,7 @@
         <v>1763.990844726562</v>
       </c>
       <c r="F257" t="n">
-        <v>1740.072265625</v>
+        <v>1740.072387695312</v>
       </c>
       <c r="G257" t="n">
         <v>16162959</v>
@@ -6381,7 +6381,7 @@
         <v>1784.804443359375</v>
       </c>
       <c r="F258" t="n">
-        <v>1760.603759765625</v>
+        <v>1760.603881835938</v>
       </c>
       <c r="G258" t="n">
         <v>13770093</v>
@@ -6404,7 +6404,7 @@
         <v>1751.1611328125</v>
       </c>
       <c r="F259" t="n">
-        <v>1727.41650390625</v>
+        <v>1727.416625976562</v>
       </c>
       <c r="G259" t="n">
         <v>16653912</v>
@@ -6427,7 +6427,7 @@
         <v>1806.356567382812</v>
       </c>
       <c r="F260" t="n">
-        <v>1781.86376953125</v>
+        <v>1781.863647460938</v>
       </c>
       <c r="G260" t="n">
         <v>20580773</v>
@@ -6588,7 +6588,7 @@
         <v>1937.745483398438</v>
       </c>
       <c r="F267" t="n">
-        <v>1911.470947265625</v>
+        <v>1911.471069335938</v>
       </c>
       <c r="G267" t="n">
         <v>19543871</v>
@@ -6634,7 +6634,7 @@
         <v>1791.542358398438</v>
       </c>
       <c r="F269" t="n">
-        <v>1767.250244140625</v>
+        <v>1767.250366210938</v>
       </c>
       <c r="G269" t="n">
         <v>27103552</v>
@@ -6657,7 +6657,7 @@
         <v>1749.084350585938</v>
       </c>
       <c r="F270" t="n">
-        <v>1725.368041992188</v>
+        <v>1725.367919921875</v>
       </c>
       <c r="G270" t="n">
         <v>21185065</v>
@@ -6680,7 +6680,7 @@
         <v>1732.055053710938</v>
       </c>
       <c r="F271" t="n">
-        <v>1708.569580078125</v>
+        <v>1708.569458007812</v>
       </c>
       <c r="G271" t="n">
         <v>17033907</v>
@@ -6749,7 +6749,7 @@
         <v>1777.512817382812</v>
       </c>
       <c r="F274" t="n">
-        <v>1753.410888671875</v>
+        <v>1753.411010742188</v>
       </c>
       <c r="G274" t="n">
         <v>20735017</v>
@@ -6795,7 +6795,7 @@
         <v>1776.128295898438</v>
       </c>
       <c r="F276" t="n">
-        <v>1752.045166015625</v>
+        <v>1752.045043945312</v>
       </c>
       <c r="G276" t="n">
         <v>12813490</v>
@@ -6864,7 +6864,7 @@
         <v>1805.525756835938</v>
       </c>
       <c r="F279" t="n">
-        <v>1781.044189453125</v>
+        <v>1781.044067382812</v>
       </c>
       <c r="G279" t="n">
         <v>9802070</v>
@@ -6933,7 +6933,7 @@
         <v>1884.396118164062</v>
       </c>
       <c r="F282" t="n">
-        <v>1858.844848632812</v>
+        <v>1858.845092773438</v>
       </c>
       <c r="G282" t="n">
         <v>15248514</v>
@@ -6956,7 +6956,7 @@
         <v>1876.089111328125</v>
       </c>
       <c r="F283" t="n">
-        <v>1850.650634765625</v>
+        <v>1850.650756835938</v>
       </c>
       <c r="G283" t="n">
         <v>7895549</v>
@@ -7002,7 +7002,7 @@
         <v>1922.839111328125</v>
       </c>
       <c r="F285" t="n">
-        <v>1896.766845703125</v>
+        <v>1896.766723632812</v>
       </c>
       <c r="G285" t="n">
         <v>11871497</v>
@@ -7025,7 +7025,7 @@
         <v>1908.486450195312</v>
       </c>
       <c r="F286" t="n">
-        <v>1882.608642578125</v>
+        <v>1882.60888671875</v>
       </c>
       <c r="G286" t="n">
         <v>9323438</v>
@@ -7117,7 +7117,7 @@
         <v>1902.302368164062</v>
       </c>
       <c r="F290" t="n">
-        <v>1876.508422851562</v>
+        <v>1876.508544921875</v>
       </c>
       <c r="G290" t="n">
         <v>5403831</v>
@@ -7140,7 +7140,7 @@
         <v>1979.234375</v>
       </c>
       <c r="F291" t="n">
-        <v>1952.397216796875</v>
+        <v>1952.397338867188</v>
       </c>
       <c r="G291" t="n">
         <v>17427846</v>
@@ -7163,7 +7163,7 @@
         <v>1925.192749023438</v>
       </c>
       <c r="F292" t="n">
-        <v>1899.088500976562</v>
+        <v>1899.08837890625</v>
       </c>
       <c r="G292" t="n">
         <v>18740607</v>
@@ -7186,7 +7186,7 @@
         <v>1939.868408203125</v>
       </c>
       <c r="F293" t="n">
-        <v>1913.565185546875</v>
+        <v>1913.565063476562</v>
       </c>
       <c r="G293" t="n">
         <v>8840382</v>
@@ -7232,7 +7232,7 @@
         <v>2032.53759765625</v>
       </c>
       <c r="F295" t="n">
-        <v>2004.977661132812</v>
+        <v>2004.977783203125</v>
       </c>
       <c r="G295" t="n">
         <v>15962230</v>
@@ -7255,7 +7255,7 @@
         <v>2008.308837890625</v>
       </c>
       <c r="F296" t="n">
-        <v>1981.077514648438</v>
+        <v>1981.07763671875</v>
       </c>
       <c r="G296" t="n">
         <v>10717877</v>
@@ -7393,7 +7393,7 @@
         <v>1946.514038085938</v>
       </c>
       <c r="F302" t="n">
-        <v>1920.12060546875</v>
+        <v>1920.120727539062</v>
       </c>
       <c r="G302" t="n">
         <v>8349049</v>
@@ -7416,7 +7416,7 @@
         <v>1938.853149414062</v>
       </c>
       <c r="F303" t="n">
-        <v>1912.563720703125</v>
+        <v>1912.563598632812</v>
       </c>
       <c r="G303" t="n">
         <v>6936900</v>
@@ -7439,7 +7439,7 @@
         <v>1897.08740234375</v>
       </c>
       <c r="F304" t="n">
-        <v>1871.364379882812</v>
+        <v>1871.364135742188</v>
       </c>
       <c r="G304" t="n">
         <v>9605118</v>
@@ -7462,7 +7462,7 @@
         <v>1854.398681640625</v>
       </c>
       <c r="F305" t="n">
-        <v>1829.254272460938</v>
+        <v>1829.25439453125</v>
       </c>
       <c r="G305" t="n">
         <v>10323740</v>
@@ -7485,7 +7485,7 @@
         <v>1921.685302734375</v>
       </c>
       <c r="F306" t="n">
-        <v>1895.628540039062</v>
+        <v>1895.628662109375</v>
       </c>
       <c r="G306" t="n">
         <v>20893714</v>
@@ -7508,7 +7508,7 @@
         <v>1903.594482421875</v>
       </c>
       <c r="F307" t="n">
-        <v>1877.783081054688</v>
+        <v>1877.783203125</v>
       </c>
       <c r="G307" t="n">
         <v>9286239</v>
@@ -7531,7 +7531,7 @@
         <v>1926.761840820312</v>
       </c>
       <c r="F308" t="n">
-        <v>1900.636352539062</v>
+        <v>1900.63623046875</v>
       </c>
       <c r="G308" t="n">
         <v>8710582</v>
@@ -7554,7 +7554,7 @@
         <v>1889.6572265625</v>
       </c>
       <c r="F309" t="n">
-        <v>1864.034912109375</v>
+        <v>1864.034790039062</v>
       </c>
       <c r="G309" t="n">
         <v>8411407</v>
@@ -7600,7 +7600,7 @@
         <v>1841.061279296875</v>
       </c>
       <c r="F311" t="n">
-        <v>1816.097778320312</v>
+        <v>1816.09765625</v>
       </c>
       <c r="G311" t="n">
         <v>10090101</v>
@@ -7715,7 +7715,7 @@
         <v>1831.50830078125</v>
       </c>
       <c r="F316" t="n">
-        <v>1806.674438476562</v>
+        <v>1806.674194335938</v>
       </c>
       <c r="G316" t="n">
         <v>7004597</v>
@@ -7784,7 +7784,7 @@
         <v>1829.431518554688</v>
       </c>
       <c r="F319" t="n">
-        <v>1804.625610351562</v>
+        <v>1804.625732421875</v>
       </c>
       <c r="G319" t="n">
         <v>7018942</v>
@@ -7807,7 +7807,7 @@
         <v>1763.990844726562</v>
       </c>
       <c r="F320" t="n">
-        <v>1740.072265625</v>
+        <v>1740.072387695312</v>
       </c>
       <c r="G320" t="n">
         <v>10450741</v>
@@ -7830,7 +7830,7 @@
         <v>1783.05078125</v>
       </c>
       <c r="F321" t="n">
-        <v>1758.873901367188</v>
+        <v>1758.873779296875</v>
       </c>
       <c r="G321" t="n">
         <v>9705594</v>
@@ -7853,7 +7853,7 @@
         <v>1794.588256835938</v>
       </c>
       <c r="F322" t="n">
-        <v>1770.2548828125</v>
+        <v>1770.255004882812</v>
       </c>
       <c r="G322" t="n">
         <v>9861858</v>
@@ -7876,7 +7876,7 @@
         <v>1783.32763671875</v>
       </c>
       <c r="F323" t="n">
-        <v>1759.14697265625</v>
+        <v>1759.147094726562</v>
       </c>
       <c r="G323" t="n">
         <v>7828474</v>
@@ -7945,7 +7945,7 @@
         <v>1759.606567382812</v>
       </c>
       <c r="F326" t="n">
-        <v>1735.747436523438</v>
+        <v>1735.74755859375</v>
       </c>
       <c r="G326" t="n">
         <v>7245477</v>
@@ -7968,7 +7968,7 @@
         <v>1757.714477539062</v>
       </c>
       <c r="F327" t="n">
-        <v>1733.881103515625</v>
+        <v>1733.881225585938</v>
       </c>
       <c r="G327" t="n">
         <v>5914428</v>
@@ -8014,7 +8014,7 @@
         <v>1835.523315429688</v>
       </c>
       <c r="F329" t="n">
-        <v>1810.634887695312</v>
+        <v>1810.634765625</v>
       </c>
       <c r="G329" t="n">
         <v>9996262</v>
@@ -8037,7 +8037,7 @@
         <v>1843.507202148438</v>
       </c>
       <c r="F330" t="n">
-        <v>1818.510375976562</v>
+        <v>1818.510620117188</v>
       </c>
       <c r="G330" t="n">
         <v>8561218</v>
@@ -8106,7 +8106,7 @@
         <v>1808.202514648438</v>
       </c>
       <c r="F333" t="n">
-        <v>1783.6845703125</v>
+        <v>1783.684692382812</v>
       </c>
       <c r="G333" t="n">
         <v>11820093</v>
@@ -8129,7 +8129,7 @@
         <v>1769.021118164062</v>
       </c>
       <c r="F334" t="n">
-        <v>1745.034423828125</v>
+        <v>1745.034545898438</v>
       </c>
       <c r="G334" t="n">
         <v>10924915</v>
@@ -8221,7 +8221,7 @@
         <v>1777.881958007812</v>
       </c>
       <c r="F338" t="n">
-        <v>1753.775268554688</v>
+        <v>1753.775146484375</v>
       </c>
       <c r="G338" t="n">
         <v>6970618</v>
@@ -8244,7 +8244,7 @@
         <v>1784.296875</v>
       </c>
       <c r="F339" t="n">
-        <v>1760.102905273438</v>
+        <v>1760.10302734375</v>
       </c>
       <c r="G339" t="n">
         <v>6739132</v>
@@ -8267,7 +8267,7 @@
         <v>1765.836791992188</v>
       </c>
       <c r="F340" t="n">
-        <v>1741.893188476562</v>
+        <v>1741.893310546875</v>
       </c>
       <c r="G340" t="n">
         <v>6588980</v>
@@ -8313,7 +8313,7 @@
         <v>1809.402465820312</v>
       </c>
       <c r="F342" t="n">
-        <v>1784.868286132812</v>
+        <v>1784.8681640625</v>
       </c>
       <c r="G342" t="n">
         <v>5936539</v>
@@ -8336,7 +8336,7 @@
         <v>1834.877197265625</v>
       </c>
       <c r="F343" t="n">
-        <v>1809.99755859375</v>
+        <v>1809.997436523438</v>
       </c>
       <c r="G343" t="n">
         <v>6032459</v>
@@ -8359,7 +8359,7 @@
         <v>1843.276489257812</v>
       </c>
       <c r="F344" t="n">
-        <v>1818.282958984375</v>
+        <v>1818.282836914062</v>
       </c>
       <c r="G344" t="n">
         <v>8158501</v>
@@ -8382,7 +8382,7 @@
         <v>1832.523559570312</v>
       </c>
       <c r="F345" t="n">
-        <v>1807.675903320312</v>
+        <v>1807.675659179688</v>
       </c>
       <c r="G345" t="n">
         <v>5711266</v>
@@ -8405,7 +8405,7 @@
         <v>1848.35302734375</v>
       </c>
       <c r="F346" t="n">
-        <v>1823.29052734375</v>
+        <v>1823.290649414062</v>
       </c>
       <c r="G346" t="n">
         <v>5392802</v>
@@ -8428,7 +8428,7 @@
         <v>1832.754272460938</v>
       </c>
       <c r="F347" t="n">
-        <v>1807.9033203125</v>
+        <v>1807.903442382812</v>
       </c>
       <c r="G347" t="n">
         <v>4275880</v>
@@ -8451,7 +8451,7 @@
         <v>1811.98681640625</v>
       </c>
       <c r="F348" t="n">
-        <v>1787.417602539062</v>
+        <v>1787.41748046875</v>
       </c>
       <c r="G348" t="n">
         <v>7390051</v>
@@ -8474,7 +8474,7 @@
         <v>1818.35546875</v>
       </c>
       <c r="F349" t="n">
-        <v>1793.69970703125</v>
+        <v>1793.699829101562</v>
       </c>
       <c r="G349" t="n">
         <v>3740102</v>
@@ -8497,7 +8497,7 @@
         <v>1823.939697265625</v>
       </c>
       <c r="F350" t="n">
-        <v>1799.20849609375</v>
+        <v>1799.208374023438</v>
       </c>
       <c r="G350" t="n">
         <v>13409647</v>
@@ -8543,7 +8543,7 @@
         <v>1993.956176757812</v>
       </c>
       <c r="F352" t="n">
-        <v>1966.919555664062</v>
+        <v>1966.91943359375</v>
       </c>
       <c r="G352" t="n">
         <v>29562071</v>
@@ -8566,7 +8566,7 @@
         <v>2001.89404296875</v>
       </c>
       <c r="F353" t="n">
-        <v>1974.749877929688</v>
+        <v>1974.749755859375</v>
       </c>
       <c r="G353" t="n">
         <v>14006916</v>
@@ -8589,7 +8589,7 @@
         <v>2031.753051757812</v>
       </c>
       <c r="F354" t="n">
-        <v>2004.203857421875</v>
+        <v>2004.203979492188</v>
       </c>
       <c r="G354" t="n">
         <v>12315081</v>
@@ -8612,7 +8612,7 @@
         <v>2039.506225585938</v>
       </c>
       <c r="F355" t="n">
-        <v>2011.851806640625</v>
+        <v>2011.851928710938</v>
       </c>
       <c r="G355" t="n">
         <v>11987128</v>
@@ -8635,7 +8635,7 @@
         <v>2021.830810546875</v>
       </c>
       <c r="F356" t="n">
-        <v>1994.416137695312</v>
+        <v>1994.416259765625</v>
       </c>
       <c r="G356" t="n">
         <v>7234323</v>
@@ -8681,7 +8681,7 @@
         <v>2044.075073242188</v>
       </c>
       <c r="F358" t="n">
-        <v>2016.35888671875</v>
+        <v>2016.359008789062</v>
       </c>
       <c r="G358" t="n">
         <v>4837367</v>
@@ -8934,7 +8934,7 @@
         <v>2035.537353515625</v>
       </c>
       <c r="F369" t="n">
-        <v>2014.936889648438</v>
+        <v>2014.93701171875</v>
       </c>
       <c r="G369" t="n">
         <v>8326975</v>
@@ -9072,7 +9072,7 @@
         <v>1936.4072265625</v>
       </c>
       <c r="F375" t="n">
-        <v>1916.810180664062</v>
+        <v>1916.81005859375</v>
       </c>
       <c r="G375" t="n">
         <v>6267203</v>
@@ -9095,7 +9095,7 @@
         <v>1965.112426757812</v>
       </c>
       <c r="F376" t="n">
-        <v>1945.224731445312</v>
+        <v>1945.224853515625</v>
       </c>
       <c r="G376" t="n">
         <v>7043310</v>
@@ -9118,7 +9118,7 @@
         <v>1984.633911132812</v>
       </c>
       <c r="F377" t="n">
-        <v>1964.548706054688</v>
+        <v>1964.548828125</v>
       </c>
       <c r="G377" t="n">
         <v>5851143</v>
@@ -9371,7 +9371,7 @@
         <v>1932.57666015625</v>
       </c>
       <c r="F388" t="n">
-        <v>1913.018188476562</v>
+        <v>1913.018310546875</v>
       </c>
       <c r="G388" t="n">
         <v>3370732</v>
@@ -9417,7 +9417,7 @@
         <v>1943.560424804688</v>
       </c>
       <c r="F390" t="n">
-        <v>1923.890991210938</v>
+        <v>1923.890869140625</v>
       </c>
       <c r="G390" t="n">
         <v>4968515</v>
@@ -9440,7 +9440,7 @@
         <v>1916.931884765625</v>
       </c>
       <c r="F391" t="n">
-        <v>1897.531982421875</v>
+        <v>1897.531860351562</v>
       </c>
       <c r="G391" t="n">
         <v>6194834</v>
@@ -9486,7 +9486,7 @@
         <v>1880.473388671875</v>
       </c>
       <c r="F393" t="n">
-        <v>1861.4423828125</v>
+        <v>1861.442260742188</v>
       </c>
       <c r="G393" t="n">
         <v>6448924</v>
@@ -9509,7 +9509,7 @@
         <v>1895.149047851562</v>
       </c>
       <c r="F394" t="n">
-        <v>1875.969482421875</v>
+        <v>1875.969360351562</v>
       </c>
       <c r="G394" t="n">
         <v>6882869</v>
@@ -9578,7 +9578,7 @@
         <v>1926.992553710938</v>
       </c>
       <c r="F397" t="n">
-        <v>1907.490600585938</v>
+        <v>1907.49072265625</v>
       </c>
       <c r="G397" t="n">
         <v>5908649</v>
@@ -9601,7 +9601,7 @@
         <v>1941.760620117188</v>
       </c>
       <c r="F398" t="n">
-        <v>1922.109252929688</v>
+        <v>1922.109375</v>
       </c>
       <c r="G398" t="n">
         <v>6584900</v>
@@ -9670,7 +9670,7 @@
         <v>1917.208740234375</v>
       </c>
       <c r="F401" t="n">
-        <v>1897.805908203125</v>
+        <v>1897.805786132812</v>
       </c>
       <c r="G401" t="n">
         <v>3747071</v>
@@ -9762,7 +9762,7 @@
         <v>1980.434204101562</v>
       </c>
       <c r="F405" t="n">
-        <v>1960.3916015625</v>
+        <v>1960.391479492188</v>
       </c>
       <c r="G405" t="n">
         <v>6390450</v>
@@ -9785,7 +9785,7 @@
         <v>2006.139770507812</v>
       </c>
       <c r="F406" t="n">
-        <v>1985.8369140625</v>
+        <v>1985.837036132812</v>
       </c>
       <c r="G406" t="n">
         <v>10967722</v>
@@ -9808,7 +9808,7 @@
         <v>1997.60205078125</v>
       </c>
       <c r="F407" t="n">
-        <v>1977.3857421875</v>
+        <v>1977.385620117188</v>
       </c>
       <c r="G407" t="n">
         <v>6329084</v>
@@ -9831,7 +9831,7 @@
         <v>2005.355224609375</v>
       </c>
       <c r="F408" t="n">
-        <v>1985.060424804688</v>
+        <v>1985.060302734375</v>
       </c>
       <c r="G408" t="n">
         <v>5037930</v>
@@ -9877,7 +9877,7 @@
         <v>1995.848388671875</v>
       </c>
       <c r="F410" t="n">
-        <v>1975.649658203125</v>
+        <v>1975.649780273438</v>
       </c>
       <c r="G410" t="n">
         <v>4927197</v>
@@ -9900,7 +9900,7 @@
         <v>2015.554443359375</v>
       </c>
       <c r="F411" t="n">
-        <v>1995.156372070312</v>
+        <v>1995.15625</v>
       </c>
       <c r="G411" t="n">
         <v>5932236</v>
@@ -10084,7 +10084,7 @@
         <v>2204.584716796875</v>
       </c>
       <c r="F419" t="n">
-        <v>2182.2734375</v>
+        <v>2182.273681640625</v>
       </c>
       <c r="G419" t="n">
         <v>15332214</v>
@@ -10107,7 +10107,7 @@
         <v>2238.828125</v>
       </c>
       <c r="F420" t="n">
-        <v>2216.17041015625</v>
+        <v>2216.170654296875</v>
       </c>
       <c r="G420" t="n">
         <v>16820855</v>
@@ -10130,7 +10130,7 @@
         <v>2252.949951171875</v>
       </c>
       <c r="F421" t="n">
-        <v>2230.149169921875</v>
+        <v>2230.1494140625</v>
       </c>
       <c r="G421" t="n">
         <v>8674941</v>
@@ -10153,7 +10153,7 @@
         <v>2244.13525390625</v>
       </c>
       <c r="F422" t="n">
-        <v>2221.423583984375</v>
+        <v>2221.423828125</v>
       </c>
       <c r="G422" t="n">
         <v>7150825</v>
@@ -10176,7 +10176,7 @@
         <v>2238.828125</v>
       </c>
       <c r="F423" t="n">
-        <v>2216.17041015625</v>
+        <v>2216.170654296875</v>
       </c>
       <c r="G423" t="n">
         <v>4481624</v>
@@ -10314,7 +10314,7 @@
         <v>2209.984375</v>
       </c>
       <c r="F429" t="n">
-        <v>2187.61865234375</v>
+        <v>2187.618408203125</v>
       </c>
       <c r="G429" t="n">
         <v>5889909</v>
@@ -10498,7 +10498,7 @@
         <v>2325.266845703125</v>
       </c>
       <c r="F437" t="n">
-        <v>2301.734130859375</v>
+        <v>2301.734375</v>
       </c>
       <c r="G437" t="n">
         <v>6795327</v>
@@ -10544,7 +10544,7 @@
         <v>2359.32568359375</v>
       </c>
       <c r="F439" t="n">
-        <v>2335.448486328125</v>
+        <v>2335.4482421875</v>
       </c>
       <c r="G439" t="n">
         <v>5459276</v>
@@ -10567,7 +10567,7 @@
         <v>2408.290771484375</v>
       </c>
       <c r="F440" t="n">
-        <v>2383.91796875</v>
+        <v>2383.918212890625</v>
       </c>
       <c r="G440" t="n">
         <v>6766817</v>
@@ -10590,7 +10590,7 @@
         <v>2362.74072265625</v>
       </c>
       <c r="F441" t="n">
-        <v>2338.8291015625</v>
+        <v>2338.828857421875</v>
       </c>
       <c r="G441" t="n">
         <v>5129440</v>
@@ -10705,7 +10705,7 @@
         <v>2487.43798828125</v>
       </c>
       <c r="F446" t="n">
-        <v>2462.26416015625</v>
+        <v>2462.264404296875</v>
       </c>
       <c r="G446" t="n">
         <v>4979881</v>
@@ -10728,7 +10728,7 @@
         <v>2492.46826171875</v>
       </c>
       <c r="F447" t="n">
-        <v>2467.243896484375</v>
+        <v>2467.24365234375</v>
       </c>
       <c r="G447" t="n">
         <v>4311734</v>
@@ -10797,7 +10797,7 @@
         <v>2492.46826171875</v>
       </c>
       <c r="F450" t="n">
-        <v>2467.243896484375</v>
+        <v>2467.24365234375</v>
       </c>
       <c r="G450" t="n">
         <v>6355285</v>
@@ -10820,7 +10820,7 @@
         <v>2420.566650390625</v>
       </c>
       <c r="F451" t="n">
-        <v>2396.06982421875</v>
+        <v>2396.069580078125</v>
       </c>
       <c r="G451" t="n">
         <v>10415834</v>
@@ -10843,7 +10843,7 @@
         <v>2425.08935546875</v>
       </c>
       <c r="F452" t="n">
-        <v>2400.546630859375</v>
+        <v>2400.54638671875</v>
       </c>
       <c r="G452" t="n">
         <v>5513737</v>
@@ -10912,7 +10912,7 @@
         <v>2425.08935546875</v>
       </c>
       <c r="F455" t="n">
-        <v>2400.546630859375</v>
+        <v>2400.54638671875</v>
       </c>
       <c r="G455" t="n">
         <v>4948149</v>
@@ -10958,7 +10958,7 @@
         <v>2340.9580078125</v>
       </c>
       <c r="F457" t="n">
-        <v>2317.266845703125</v>
+        <v>2317.2666015625</v>
       </c>
       <c r="G457" t="n">
         <v>7116512</v>
@@ -10981,7 +10981,7 @@
         <v>2342.388671875</v>
       </c>
       <c r="F458" t="n">
-        <v>2318.682861328125</v>
+        <v>2318.68310546875</v>
       </c>
       <c r="G458" t="n">
         <v>7740557</v>
@@ -11234,7 +11234,7 @@
         <v>2274.271240234375</v>
       </c>
       <c r="F469" t="n">
-        <v>2251.2548828125</v>
+        <v>2251.255126953125</v>
       </c>
       <c r="G469" t="n">
         <v>5101014</v>
@@ -11326,7 +11326,7 @@
         <v>2170.341552734375</v>
       </c>
       <c r="F473" t="n">
-        <v>2148.376708984375</v>
+        <v>2148.376953125</v>
       </c>
       <c r="G473" t="n">
         <v>8410148</v>
@@ -11418,7 +11418,7 @@
         <v>2220.183349609375</v>
       </c>
       <c r="F477" t="n">
-        <v>2197.714111328125</v>
+        <v>2197.71435546875</v>
       </c>
       <c r="G477" t="n">
         <v>16086149</v>
@@ -11556,7 +11556,7 @@
         <v>2231.905517578125</v>
       </c>
       <c r="F483" t="n">
-        <v>2209.318115234375</v>
+        <v>2209.31787109375</v>
       </c>
       <c r="G483" t="n">
         <v>4372089</v>
@@ -11740,7 +11740,7 @@
         <v>2101.993408203125</v>
       </c>
       <c r="F491" t="n">
-        <v>2080.72021484375</v>
+        <v>2080.720458984375</v>
       </c>
       <c r="G491" t="n">
         <v>7162923</v>
@@ -11878,7 +11878,7 @@
         <v>2213.722412109375</v>
       </c>
       <c r="F497" t="n">
-        <v>2191.318603515625</v>
+        <v>2191.31884765625</v>
       </c>
       <c r="G497" t="n">
         <v>3187306</v>
@@ -12016,7 +12016,7 @@
         <v>2279.43994140625</v>
       </c>
       <c r="F503" t="n">
-        <v>2256.371337890625</v>
+        <v>2256.37109375</v>
       </c>
       <c r="G503" t="n">
         <v>5821906</v>
@@ -12039,7 +12039,7 @@
         <v>2230.4287109375</v>
       </c>
       <c r="F504" t="n">
-        <v>2207.85595703125</v>
+        <v>2207.856201171875</v>
       </c>
       <c r="G504" t="n">
         <v>7223711</v>
@@ -12062,7 +12062,7 @@
         <v>2248.42724609375</v>
       </c>
       <c r="F505" t="n">
-        <v>2225.67236328125</v>
+        <v>2225.672607421875</v>
       </c>
       <c r="G505" t="n">
         <v>6556057</v>
@@ -12085,7 +12085,7 @@
         <v>2250.273193359375</v>
       </c>
       <c r="F506" t="n">
-        <v>2227.499755859375</v>
+        <v>2227.49951171875</v>
       </c>
       <c r="G506" t="n">
         <v>4623365</v>
@@ -12131,7 +12131,7 @@
         <v>2326.974365234375</v>
       </c>
       <c r="F508" t="n">
-        <v>2303.424560546875</v>
+        <v>2303.42431640625</v>
       </c>
       <c r="G508" t="n">
         <v>7400221</v>
@@ -12177,7 +12177,7 @@
         <v>2343.49609375</v>
       </c>
       <c r="F510" t="n">
-        <v>2319.77880859375</v>
+        <v>2319.779052734375</v>
       </c>
       <c r="G510" t="n">
         <v>9965088</v>
@@ -12269,7 +12269,7 @@
         <v>2286.685546875</v>
       </c>
       <c r="F514" t="n">
-        <v>2263.543701171875</v>
+        <v>2263.54345703125</v>
       </c>
       <c r="G514" t="n">
         <v>8247243</v>
@@ -12384,7 +12384,7 @@
         <v>2155.98876953125</v>
       </c>
       <c r="F519" t="n">
-        <v>2134.16943359375</v>
+        <v>2134.169189453125</v>
       </c>
       <c r="G519" t="n">
         <v>7333863</v>
@@ -12453,7 +12453,7 @@
         <v>2200.015869140625</v>
       </c>
       <c r="F522" t="n">
-        <v>2177.750732421875</v>
+        <v>2177.7509765625</v>
       </c>
       <c r="G522" t="n">
         <v>5008845</v>
@@ -12476,7 +12476,7 @@
         <v>2171.58740234375</v>
       </c>
       <c r="F523" t="n">
-        <v>2149.6103515625</v>
+        <v>2149.610107421875</v>
       </c>
       <c r="G523" t="n">
         <v>4786419</v>
@@ -12499,7 +12499,7 @@
         <v>2151.7890625</v>
       </c>
       <c r="F524" t="n">
-        <v>2130.01220703125</v>
+        <v>2130.012451171875</v>
       </c>
       <c r="G524" t="n">
         <v>5530620</v>
@@ -12614,7 +12614,7 @@
         <v>2193.41650390625</v>
       </c>
       <c r="F529" t="n">
-        <v>2171.218505859375</v>
+        <v>2171.21826171875</v>
       </c>
       <c r="G529" t="n">
         <v>7971685</v>
@@ -12637,7 +12637,7 @@
         <v>2158.48095703125</v>
       </c>
       <c r="F530" t="n">
-        <v>2136.636474609375</v>
+        <v>2136.63623046875</v>
       </c>
       <c r="G530" t="n">
         <v>5359816</v>
@@ -12660,7 +12660,7 @@
         <v>2231.76708984375</v>
       </c>
       <c r="F531" t="n">
-        <v>2209.180908203125</v>
+        <v>2209.1806640625</v>
       </c>
       <c r="G531" t="n">
         <v>5606335</v>
@@ -12706,7 +12706,7 @@
         <v>2255.349609375</v>
       </c>
       <c r="F533" t="n">
-        <v>2232.52490234375</v>
+        <v>2232.524658203125</v>
       </c>
       <c r="G533" t="n">
         <v>6426626</v>
@@ -12890,7 +12890,7 @@
         <v>2213.86083984375</v>
       </c>
       <c r="F541" t="n">
-        <v>2191.455810546875</v>
+        <v>2191.4560546875</v>
       </c>
       <c r="G541" t="n">
         <v>10735893</v>
@@ -12959,7 +12959,7 @@
         <v>2067.10400390625</v>
       </c>
       <c r="F544" t="n">
-        <v>2046.184326171875</v>
+        <v>2046.184204101562</v>
       </c>
       <c r="G544" t="n">
         <v>8991655</v>
@@ -13074,7 +13074,7 @@
         <v>2232.59765625</v>
       </c>
       <c r="F549" t="n">
-        <v>2210.003173828125</v>
+        <v>2210.0029296875</v>
       </c>
       <c r="G549" t="n">
         <v>4170339</v>
@@ -13120,7 +13120,7 @@
         <v>2218.291259765625</v>
       </c>
       <c r="F551" t="n">
-        <v>2195.841552734375</v>
+        <v>2195.84130859375</v>
       </c>
       <c r="G551" t="n">
         <v>5574914</v>
@@ -13143,7 +13143,7 @@
         <v>2290.6083984375</v>
       </c>
       <c r="F552" t="n">
-        <v>2267.426513671875</v>
+        <v>2267.4267578125</v>
       </c>
       <c r="G552" t="n">
         <v>10711049</v>
@@ -13166,7 +13166,7 @@
         <v>2277.409423828125</v>
       </c>
       <c r="F553" t="n">
-        <v>2254.361328125</v>
+        <v>2254.361083984375</v>
       </c>
       <c r="G553" t="n">
         <v>5999733</v>
@@ -13212,7 +13212,7 @@
         <v>2343.6806640625</v>
       </c>
       <c r="F555" t="n">
-        <v>2319.9619140625</v>
+        <v>2319.961669921875</v>
       </c>
       <c r="G555" t="n">
         <v>7731093</v>
@@ -13235,7 +13235,7 @@
         <v>2380.093017578125</v>
       </c>
       <c r="F556" t="n">
-        <v>2356.00537109375</v>
+        <v>2356.005615234375</v>
       </c>
       <c r="G556" t="n">
         <v>6584133</v>
@@ -13327,7 +13327,7 @@
         <v>2467.132080078125</v>
       </c>
       <c r="F560" t="n">
-        <v>2442.1640625</v>
+        <v>2442.163818359375</v>
       </c>
       <c r="G560" t="n">
         <v>7905775</v>
@@ -13373,7 +13373,7 @@
         <v>2451.3486328125</v>
       </c>
       <c r="F562" t="n">
-        <v>2426.540283203125</v>
+        <v>2426.5400390625</v>
       </c>
       <c r="G562" t="n">
         <v>3961440</v>
@@ -13419,7 +13419,7 @@
         <v>2423.84326171875</v>
       </c>
       <c r="F564" t="n">
-        <v>2399.313232421875</v>
+        <v>2399.31298828125</v>
       </c>
       <c r="G564" t="n">
         <v>6574935</v>
@@ -13580,7 +13580,7 @@
         <v>2347.97265625</v>
       </c>
       <c r="F571" t="n">
-        <v>2324.210205078125</v>
+        <v>2324.21044921875</v>
       </c>
       <c r="G571" t="n">
         <v>4987112</v>
@@ -13626,7 +13626,7 @@
         <v>2509.12841796875</v>
       </c>
       <c r="F573" t="n">
-        <v>2483.735107421875</v>
+        <v>2483.7353515625</v>
       </c>
       <c r="G573" t="n">
         <v>12536120</v>
@@ -13718,7 +13718,7 @@
         <v>2561.924072265625</v>
       </c>
       <c r="F577" t="n">
-        <v>2535.99658203125</v>
+        <v>2535.996337890625</v>
       </c>
       <c r="G577" t="n">
         <v>6113833</v>
@@ -13810,7 +13810,7 @@
         <v>2566.3544921875</v>
       </c>
       <c r="F581" t="n">
-        <v>2540.382080078125</v>
+        <v>2540.38232421875</v>
       </c>
       <c r="G581" t="n">
         <v>4733503</v>
@@ -13833,7 +13833,7 @@
         <v>2486.238037109375</v>
       </c>
       <c r="F582" t="n">
-        <v>2461.076416015625</v>
+        <v>2461.07666015625</v>
       </c>
       <c r="G582" t="n">
         <v>9623830</v>
@@ -13948,7 +13948,7 @@
         <v>2260.703125</v>
       </c>
       <c r="F587" t="n">
-        <v>2237.823974609375</v>
+        <v>2237.82421875</v>
       </c>
       <c r="G587" t="n">
         <v>8321949</v>
@@ -13971,7 +13971,7 @@
         <v>2214.6455078125</v>
       </c>
       <c r="F588" t="n">
-        <v>2192.232666015625</v>
+        <v>2192.232421875</v>
       </c>
       <c r="G588" t="n">
         <v>10245160</v>
@@ -14017,7 +14017,7 @@
         <v>2240.304931640625</v>
       </c>
       <c r="F590" t="n">
-        <v>2217.632080078125</v>
+        <v>2217.63232421875</v>
       </c>
       <c r="G590" t="n">
         <v>6718955</v>
@@ -14040,7 +14040,7 @@
         <v>2334.404541015625</v>
       </c>
       <c r="F591" t="n">
-        <v>2310.779541015625</v>
+        <v>2310.779296875</v>
       </c>
       <c r="G591" t="n">
         <v>8275914</v>
@@ -14178,7 +14178,7 @@
         <v>2410.875244140625</v>
       </c>
       <c r="F597" t="n">
-        <v>2386.476318359375</v>
+        <v>2386.4765625</v>
       </c>
       <c r="G597" t="n">
         <v>6357272</v>
@@ -14201,7 +14201,7 @@
         <v>2387.892578125</v>
       </c>
       <c r="F598" t="n">
-        <v>2363.72607421875</v>
+        <v>2363.726318359375</v>
       </c>
       <c r="G598" t="n">
         <v>8941011</v>
@@ -14293,7 +14293,7 @@
         <v>2430.7197265625</v>
       </c>
       <c r="F602" t="n">
-        <v>2406.119873046875</v>
+        <v>2406.1201171875</v>
       </c>
       <c r="G602" t="n">
         <v>4888494</v>
@@ -14316,7 +14316,7 @@
         <v>2514.528076171875</v>
       </c>
       <c r="F603" t="n">
-        <v>2489.080322265625</v>
+        <v>2489.080078125</v>
       </c>
       <c r="G603" t="n">
         <v>11063284</v>
@@ -14385,7 +14385,7 @@
         <v>2559.247314453125</v>
       </c>
       <c r="F606" t="n">
-        <v>2533.3466796875</v>
+        <v>2533.346923828125</v>
       </c>
       <c r="G606" t="n">
         <v>6179127</v>
@@ -14477,7 +14477,7 @@
         <v>2457.855712890625</v>
       </c>
       <c r="F610" t="n">
-        <v>2432.981201171875</v>
+        <v>2432.9814453125</v>
       </c>
       <c r="G610" t="n">
         <v>8810401</v>
@@ -14546,7 +14546,7 @@
         <v>2362.879150390625</v>
       </c>
       <c r="F613" t="n">
-        <v>2338.966064453125</v>
+        <v>2338.9658203125</v>
       </c>
       <c r="G613" t="n">
         <v>8555737</v>
@@ -14592,7 +14592,7 @@
         <v>2347.234375</v>
       </c>
       <c r="F615" t="n">
-        <v>2323.479736328125</v>
+        <v>2323.4794921875</v>
       </c>
       <c r="G615" t="n">
         <v>6033398</v>
@@ -14684,7 +14684,7 @@
         <v>2307.54541015625</v>
       </c>
       <c r="F619" t="n">
-        <v>2284.1923828125</v>
+        <v>2284.192138671875</v>
       </c>
       <c r="G619" t="n">
         <v>7120117</v>
@@ -14707,7 +14707,7 @@
         <v>2300.715087890625</v>
       </c>
       <c r="F620" t="n">
-        <v>2277.430908203125</v>
+        <v>2277.43115234375</v>
       </c>
       <c r="G620" t="n">
         <v>7737264</v>
@@ -14914,7 +14914,7 @@
         <v>2207.261474609375</v>
       </c>
       <c r="F629" t="n">
-        <v>2184.92333984375</v>
+        <v>2184.923095703125</v>
       </c>
       <c r="G629" t="n">
         <v>9505054</v>
@@ -14937,7 +14937,7 @@
         <v>2237.259033203125</v>
       </c>
       <c r="F630" t="n">
-        <v>2214.6171875</v>
+        <v>2214.616943359375</v>
       </c>
       <c r="G630" t="n">
         <v>6923733</v>
@@ -14960,7 +14960,7 @@
         <v>2234.074462890625</v>
       </c>
       <c r="F631" t="n">
-        <v>2211.46484375</v>
+        <v>2211.464599609375</v>
       </c>
       <c r="G631" t="n">
         <v>5389494</v>
@@ -14983,7 +14983,7 @@
         <v>2194.477783203125</v>
       </c>
       <c r="F632" t="n">
-        <v>2172.26904296875</v>
+        <v>2172.268798828125</v>
       </c>
       <c r="G632" t="n">
         <v>7112066</v>
@@ -15006,7 +15006,7 @@
         <v>2212.568603515625</v>
       </c>
       <c r="F633" t="n">
-        <v>2190.1767578125</v>
+        <v>2190.176513671875</v>
       </c>
       <c r="G633" t="n">
         <v>8485157</v>
@@ -15029,7 +15029,7 @@
         <v>2216.860595703125</v>
       </c>
       <c r="F634" t="n">
-        <v>2194.42529296875</v>
+        <v>2194.425048828125</v>
       </c>
       <c r="G634" t="n">
         <v>4801605</v>
@@ -15052,7 +15052,7 @@
         <v>2235.736083984375</v>
       </c>
       <c r="F635" t="n">
-        <v>2213.109619140625</v>
+        <v>2213.109375</v>
       </c>
       <c r="G635" t="n">
         <v>7580454</v>
@@ -15213,7 +15213,7 @@
         <v>2232.9208984375</v>
       </c>
       <c r="F642" t="n">
-        <v>2210.32275390625</v>
+        <v>2210.322998046875</v>
       </c>
       <c r="G642" t="n">
         <v>4327543</v>
@@ -15259,7 +15259,7 @@
         <v>2316.221435546875</v>
       </c>
       <c r="F644" t="n">
-        <v>2292.7802734375</v>
+        <v>2292.780517578125</v>
       </c>
       <c r="G644" t="n">
         <v>7565341</v>
@@ -15305,7 +15305,7 @@
         <v>2385.631103515625</v>
       </c>
       <c r="F646" t="n">
-        <v>2361.48779296875</v>
+        <v>2361.487548828125</v>
       </c>
       <c r="G646" t="n">
         <v>6958956</v>
@@ -15420,7 +15420,7 @@
         <v>2383.646728515625</v>
       </c>
       <c r="F651" t="n">
-        <v>2359.523193359375</v>
+        <v>2359.5234375</v>
       </c>
       <c r="G651" t="n">
         <v>5362344</v>
@@ -15466,7 +15466,7 @@
         <v>2430.258056640625</v>
       </c>
       <c r="F653" t="n">
-        <v>2405.6630859375</v>
+        <v>2405.662841796875</v>
       </c>
       <c r="G653" t="n">
         <v>6325293</v>
@@ -27233,19 +27233,111 @@
         <v>2914</v>
       </c>
       <c r="C1165" t="n">
-        <v>2949.89990234375</v>
+        <v>2972</v>
       </c>
       <c r="D1165" t="n">
         <v>2891.75</v>
       </c>
       <c r="E1165" t="n">
-        <v>2947</v>
+        <v>2959.60009765625</v>
       </c>
       <c r="F1165" t="n">
-        <v>2947</v>
+        <v>2959.60009765625</v>
       </c>
       <c r="G1165" t="n">
-        <v>6610010</v>
+        <v>11174688</v>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" s="2" t="n">
+        <v>45548</v>
+      </c>
+      <c r="B1166" t="n">
+        <v>2952.800048828125</v>
+      </c>
+      <c r="C1166" t="n">
+        <v>2966.300048828125</v>
+      </c>
+      <c r="D1166" t="n">
+        <v>2939</v>
+      </c>
+      <c r="E1166" t="n">
+        <v>2945.25</v>
+      </c>
+      <c r="F1166" t="n">
+        <v>2945.25</v>
+      </c>
+      <c r="G1166" t="n">
+        <v>4355664</v>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" s="2" t="n">
+        <v>45551</v>
+      </c>
+      <c r="B1167" t="n">
+        <v>2955.10009765625</v>
+      </c>
+      <c r="C1167" t="n">
+        <v>2961.800048828125</v>
+      </c>
+      <c r="D1167" t="n">
+        <v>2929.5</v>
+      </c>
+      <c r="E1167" t="n">
+        <v>2942.699951171875</v>
+      </c>
+      <c r="F1167" t="n">
+        <v>2942.699951171875</v>
+      </c>
+      <c r="G1167" t="n">
+        <v>2740887</v>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" s="2" t="n">
+        <v>45552</v>
+      </c>
+      <c r="B1168" t="n">
+        <v>2948</v>
+      </c>
+      <c r="C1168" t="n">
+        <v>2954.949951171875</v>
+      </c>
+      <c r="D1168" t="n">
+        <v>2933.25</v>
+      </c>
+      <c r="E1168" t="n">
+        <v>2944.60009765625</v>
+      </c>
+      <c r="F1168" t="n">
+        <v>2944.60009765625</v>
+      </c>
+      <c r="G1168" t="n">
+        <v>2967664</v>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" s="2" t="n">
+        <v>45553</v>
+      </c>
+      <c r="B1169" t="n">
+        <v>2940</v>
+      </c>
+      <c r="C1169" t="n">
+        <v>2951</v>
+      </c>
+      <c r="D1169" t="n">
+        <v>2937.5</v>
+      </c>
+      <c r="E1169" t="n">
+        <v>2949.050048828125</v>
+      </c>
+      <c r="F1169" t="n">
+        <v>2949.050048828125</v>
+      </c>
+      <c r="G1169" t="n">
+        <v>274791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
29 / 09 / 2024
</commit_message>
<xml_diff>
--- a/Data/reliance.xlsx
+++ b/Data/reliance.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1169"/>
+  <dimension ref="A1:G1165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
         <v>1380.276611328125</v>
       </c>
       <c r="F2" t="n">
-        <v>1356.042724609375</v>
+        <v>1356.042846679688</v>
       </c>
       <c r="G2" t="n">
         <v>7002234</v>
@@ -562,7 +562,7 @@
         <v>1372.87060546875</v>
       </c>
       <c r="F5" t="n">
-        <v>1348.766845703125</v>
+        <v>1348.766723632812</v>
       </c>
       <c r="G5" t="n">
         <v>12259588</v>
@@ -608,7 +608,7 @@
         <v>1383.522583007812</v>
       </c>
       <c r="F7" t="n">
-        <v>1359.231811523438</v>
+        <v>1359.231689453125</v>
       </c>
       <c r="G7" t="n">
         <v>8023951</v>
@@ -631,7 +631,7 @@
         <v>1415.387084960938</v>
       </c>
       <c r="F8" t="n">
-        <v>1390.536865234375</v>
+        <v>1390.536743164062</v>
       </c>
       <c r="G8" t="n">
         <v>7491371</v>
@@ -700,7 +700,7 @@
         <v>1398.380493164062</v>
       </c>
       <c r="F11" t="n">
-        <v>1373.828735351562</v>
+        <v>1373.828979492188</v>
       </c>
       <c r="G11" t="n">
         <v>7908267</v>
@@ -723,7 +723,7 @@
         <v>1393.305908203125</v>
       </c>
       <c r="F12" t="n">
-        <v>1368.843383789062</v>
+        <v>1368.84326171875</v>
       </c>
       <c r="G12" t="n">
         <v>7908929</v>
@@ -769,7 +769,7 @@
         <v>1445.56005859375</v>
       </c>
       <c r="F14" t="n">
-        <v>1420.179809570312</v>
+        <v>1420.179931640625</v>
       </c>
       <c r="G14" t="n">
         <v>14731735</v>
@@ -815,7 +815,7 @@
         <v>1402.494995117188</v>
       </c>
       <c r="F16" t="n">
-        <v>1377.871215820312</v>
+        <v>1377.87109375</v>
       </c>
       <c r="G16" t="n">
         <v>9461360</v>
@@ -838,7 +838,7 @@
         <v>1401.992065429688</v>
       </c>
       <c r="F17" t="n">
-        <v>1377.376953125</v>
+        <v>1377.377075195312</v>
       </c>
       <c r="G17" t="n">
         <v>5161408</v>
@@ -861,7 +861,7 @@
         <v>1396.048950195312</v>
       </c>
       <c r="F18" t="n">
-        <v>1371.538330078125</v>
+        <v>1371.538208007812</v>
       </c>
       <c r="G18" t="n">
         <v>5623869</v>
@@ -884,7 +884,7 @@
         <v>1391.203002929688</v>
       </c>
       <c r="F19" t="n">
-        <v>1366.777221679688</v>
+        <v>1366.77734375</v>
       </c>
       <c r="G19" t="n">
         <v>7314222</v>
@@ -930,7 +930,7 @@
         <v>1345.669189453125</v>
       </c>
       <c r="F21" t="n">
-        <v>1322.04296875</v>
+        <v>1322.042846679688</v>
       </c>
       <c r="G21" t="n">
         <v>12266118</v>
@@ -999,7 +999,7 @@
         <v>1290.7177734375</v>
       </c>
       <c r="F24" t="n">
-        <v>1268.056396484375</v>
+        <v>1268.056518554688</v>
       </c>
       <c r="G24" t="n">
         <v>17375155</v>
@@ -1091,7 +1091,7 @@
         <v>1332.914184570312</v>
       </c>
       <c r="F28" t="n">
-        <v>1309.511840820312</v>
+        <v>1309.511962890625</v>
       </c>
       <c r="G28" t="n">
         <v>7769288</v>
@@ -1160,7 +1160,7 @@
         <v>1328.296875</v>
       </c>
       <c r="F31" t="n">
-        <v>1304.9755859375</v>
+        <v>1304.975708007812</v>
       </c>
       <c r="G31" t="n">
         <v>6999908</v>
@@ -1252,7 +1252,7 @@
         <v>1351.6123046875</v>
       </c>
       <c r="F35" t="n">
-        <v>1327.881713867188</v>
+        <v>1327.8818359375</v>
       </c>
       <c r="G35" t="n">
         <v>6574565</v>
@@ -1275,7 +1275,7 @@
         <v>1341.691772460938</v>
       </c>
       <c r="F36" t="n">
-        <v>1318.135498046875</v>
+        <v>1318.13525390625</v>
       </c>
       <c r="G36" t="n">
         <v>5563580</v>
@@ -1367,7 +1367,7 @@
         <v>1295.060913085938</v>
       </c>
       <c r="F40" t="n">
-        <v>1272.323120117188</v>
+        <v>1272.3232421875</v>
       </c>
       <c r="G40" t="n">
         <v>13872531</v>
@@ -1482,7 +1482,7 @@
         <v>1227.811645507812</v>
       </c>
       <c r="F45" t="n">
-        <v>1206.254638671875</v>
+        <v>1206.254760742188</v>
       </c>
       <c r="G45" t="n">
         <v>13699399</v>
@@ -1528,7 +1528,7 @@
         <v>1198.827392578125</v>
       </c>
       <c r="F47" t="n">
-        <v>1177.779296875</v>
+        <v>1177.779174804688</v>
       </c>
       <c r="G47" t="n">
         <v>15255195</v>
@@ -1551,7 +1551,7 @@
         <v>1162.116821289062</v>
       </c>
       <c r="F48" t="n">
-        <v>1141.71337890625</v>
+        <v>1141.713256835938</v>
       </c>
       <c r="G48" t="n">
         <v>16867019</v>
@@ -1574,7 +1574,7 @@
         <v>1018.703796386719</v>
       </c>
       <c r="F49" t="n">
-        <v>1000.818176269531</v>
+        <v>1000.818237304688</v>
       </c>
       <c r="G49" t="n">
         <v>44093509</v>
@@ -1597,7 +1597,7 @@
         <v>1054.728515625</v>
       </c>
       <c r="F50" t="n">
-        <v>1036.21044921875</v>
+        <v>1036.210327148438</v>
       </c>
       <c r="G50" t="n">
         <v>29789288</v>
@@ -1689,7 +1689,7 @@
         <v>921.6473999023438</v>
       </c>
       <c r="F54" t="n">
-        <v>905.4658203125</v>
+        <v>905.4657592773438</v>
       </c>
       <c r="G54" t="n">
         <v>22722989</v>
@@ -1735,7 +1735,7 @@
         <v>839.0831298828125</v>
       </c>
       <c r="F56" t="n">
-        <v>824.35107421875</v>
+        <v>824.3511352539062</v>
       </c>
       <c r="G56" t="n">
         <v>30702005</v>
@@ -1781,7 +1781,7 @@
         <v>808.3158569335938</v>
       </c>
       <c r="F58" t="n">
-        <v>794.1241455078125</v>
+        <v>794.1240844726562</v>
       </c>
       <c r="G58" t="n">
         <v>20335474</v>
@@ -1804,7 +1804,7 @@
         <v>862.5814819335938</v>
       </c>
       <c r="F59" t="n">
-        <v>847.4369506835938</v>
+        <v>847.4368896484375</v>
       </c>
       <c r="G59" t="n">
         <v>22867443</v>
@@ -1827,7 +1827,7 @@
         <v>989.5365600585938</v>
       </c>
       <c r="F60" t="n">
-        <v>972.1630249023438</v>
+        <v>972.1630859375</v>
       </c>
       <c r="G60" t="n">
         <v>36565149</v>
@@ -1850,7 +1850,7 @@
         <v>974.8615112304688</v>
       </c>
       <c r="F61" t="n">
-        <v>957.7456665039062</v>
+        <v>957.74560546875</v>
       </c>
       <c r="G61" t="n">
         <v>22872244</v>
@@ -1873,7 +1873,7 @@
         <v>974.3129272460938</v>
       </c>
       <c r="F62" t="n">
-        <v>957.2066650390625</v>
+        <v>957.206787109375</v>
       </c>
       <c r="G62" t="n">
         <v>20828970</v>
@@ -1919,7 +1919,7 @@
         <v>1018.338073730469</v>
       </c>
       <c r="F64" t="n">
-        <v>1000.458923339844</v>
+        <v>1000.458862304688</v>
       </c>
       <c r="G64" t="n">
         <v>22146405</v>
@@ -1942,7 +1942,7 @@
         <v>987.8908081054688</v>
       </c>
       <c r="F65" t="n">
-        <v>970.5460815429688</v>
+        <v>970.546142578125</v>
       </c>
       <c r="G65" t="n">
         <v>20798729</v>
@@ -1988,7 +1988,7 @@
         <v>1102.776733398438</v>
       </c>
       <c r="F67" t="n">
-        <v>1083.4150390625</v>
+        <v>1083.415161132812</v>
       </c>
       <c r="G67" t="n">
         <v>27186812</v>
@@ -2011,7 +2011,7 @@
         <v>1090.021728515625</v>
       </c>
       <c r="F68" t="n">
-        <v>1070.883911132812</v>
+        <v>1070.884033203125</v>
       </c>
       <c r="G68" t="n">
         <v>24940165</v>
@@ -2057,7 +2057,7 @@
         <v>1087.27880859375</v>
       </c>
       <c r="F70" t="n">
-        <v>1068.189331054688</v>
+        <v>1068.189208984375</v>
       </c>
       <c r="G70" t="n">
         <v>11836892</v>
@@ -2103,7 +2103,7 @@
         <v>1067.986328125</v>
       </c>
       <c r="F72" t="n">
-        <v>1049.235229492188</v>
+        <v>1049.2353515625</v>
       </c>
       <c r="G72" t="n">
         <v>18727853</v>
@@ -2149,7 +2149,7 @@
         <v>1137.2470703125</v>
       </c>
       <c r="F74" t="n">
-        <v>1117.280151367188</v>
+        <v>1117.280029296875</v>
       </c>
       <c r="G74" t="n">
         <v>18015466</v>
@@ -2172,7 +2172,7 @@
         <v>1131.349609375</v>
       </c>
       <c r="F75" t="n">
-        <v>1111.486328125</v>
+        <v>1111.486206054688</v>
       </c>
       <c r="G75" t="n">
         <v>30685814</v>
@@ -2218,7 +2218,7 @@
         <v>1253.458740234375</v>
       </c>
       <c r="F77" t="n">
-        <v>1231.451538085938</v>
+        <v>1231.451416015625</v>
       </c>
       <c r="G77" t="n">
         <v>32732251</v>
@@ -2241,7 +2241,7 @@
         <v>1295.609497070312</v>
       </c>
       <c r="F78" t="n">
-        <v>1272.8623046875</v>
+        <v>1272.862182617188</v>
       </c>
       <c r="G78" t="n">
         <v>67493154</v>
@@ -2264,7 +2264,7 @@
         <v>1307.267211914062</v>
       </c>
       <c r="F79" t="n">
-        <v>1284.315185546875</v>
+        <v>1284.315307617188</v>
       </c>
       <c r="G79" t="n">
         <v>29241450</v>
@@ -2287,7 +2287,7 @@
         <v>1305.804321289062</v>
       </c>
       <c r="F80" t="n">
-        <v>1282.878173828125</v>
+        <v>1282.878051757812</v>
       </c>
       <c r="G80" t="n">
         <v>39226700</v>
@@ -2333,7 +2333,7 @@
         <v>1340.411743164062</v>
       </c>
       <c r="F82" t="n">
-        <v>1316.8779296875</v>
+        <v>1316.877807617188</v>
       </c>
       <c r="G82" t="n">
         <v>35672949</v>
@@ -2379,7 +2379,7 @@
         <v>1335.52001953125</v>
       </c>
       <c r="F84" t="n">
-        <v>1312.072021484375</v>
+        <v>1312.071899414062</v>
       </c>
       <c r="G84" t="n">
         <v>22451881</v>
@@ -2425,7 +2425,7 @@
         <v>1377.853637695312</v>
       </c>
       <c r="F86" t="n">
-        <v>1353.662231445312</v>
+        <v>1353.662353515625</v>
       </c>
       <c r="G86" t="n">
         <v>25013483</v>
@@ -2517,7 +2517,7 @@
         <v>1381.222900390625</v>
       </c>
       <c r="F90" t="n">
-        <v>1356.972534179688</v>
+        <v>1356.972412109375</v>
       </c>
       <c r="G90" t="n">
         <v>33215062</v>
@@ -2540,7 +2540,7 @@
         <v>1325.38134765625</v>
       </c>
       <c r="F91" t="n">
-        <v>1302.111328125</v>
+        <v>1302.111206054688</v>
       </c>
       <c r="G91" t="n">
         <v>24633385</v>
@@ -2563,7 +2563,7 @@
         <v>1347.025756835938</v>
       </c>
       <c r="F92" t="n">
-        <v>1323.375732421875</v>
+        <v>1323.375854492188</v>
       </c>
       <c r="G92" t="n">
         <v>31076130</v>
@@ -2701,7 +2701,7 @@
         <v>1314.397705078125</v>
       </c>
       <c r="F98" t="n">
-        <v>1291.320434570312</v>
+        <v>1291.320556640625</v>
       </c>
       <c r="G98" t="n">
         <v>16608317</v>
@@ -2747,7 +2747,7 @@
         <v>1358.88623046875</v>
       </c>
       <c r="F100" t="n">
-        <v>1335.02783203125</v>
+        <v>1335.027954101562</v>
       </c>
       <c r="G100" t="n">
         <v>20063139</v>
@@ -2770,7 +2770,7 @@
         <v>1351.640747070312</v>
       </c>
       <c r="F101" t="n">
-        <v>1327.909545898438</v>
+        <v>1327.90966796875</v>
       </c>
       <c r="G101" t="n">
         <v>20011263</v>
@@ -2816,7 +2816,7 @@
         <v>1417.450561523438</v>
       </c>
       <c r="F103" t="n">
-        <v>1392.56396484375</v>
+        <v>1392.564086914062</v>
       </c>
       <c r="G103" t="n">
         <v>11076980</v>
@@ -2862,7 +2862,7 @@
         <v>1458.154907226562</v>
       </c>
       <c r="F105" t="n">
-        <v>1432.553833007812</v>
+        <v>1432.5537109375</v>
       </c>
       <c r="G105" t="n">
         <v>17101175</v>
@@ -2954,7 +2954,7 @@
         <v>1451.093994140625</v>
       </c>
       <c r="F109" t="n">
-        <v>1425.616821289062</v>
+        <v>1425.61669921875</v>
       </c>
       <c r="G109" t="n">
         <v>11066323</v>
@@ -3000,7 +3000,7 @@
         <v>1466.4619140625</v>
       </c>
       <c r="F111" t="n">
-        <v>1440.714965820312</v>
+        <v>1440.71484375</v>
       </c>
       <c r="G111" t="n">
         <v>19274449</v>
@@ -3023,7 +3023,7 @@
         <v>1490.229125976562</v>
       </c>
       <c r="F112" t="n">
-        <v>1464.064819335938</v>
+        <v>1464.06494140625</v>
       </c>
       <c r="G112" t="n">
         <v>26553701</v>
@@ -3161,7 +3161,7 @@
         <v>1588.39013671875</v>
       </c>
       <c r="F118" t="n">
-        <v>1560.502319335938</v>
+        <v>1560.502563476562</v>
       </c>
       <c r="G118" t="n">
         <v>18981039</v>
@@ -3184,7 +3184,7 @@
         <v>1594.804931640625</v>
       </c>
       <c r="F119" t="n">
-        <v>1566.804565429688</v>
+        <v>1566.804809570312</v>
       </c>
       <c r="G119" t="n">
         <v>25793110</v>
@@ -3276,7 +3276,7 @@
         <v>1572.8837890625</v>
       </c>
       <c r="F123" t="n">
-        <v>1545.268432617188</v>
+        <v>1545.268310546875</v>
       </c>
       <c r="G123" t="n">
         <v>15138210</v>
@@ -3483,7 +3483,7 @@
         <v>1786.00439453125</v>
       </c>
       <c r="F132" t="n">
-        <v>1761.787353515625</v>
+        <v>1761.787475585938</v>
       </c>
       <c r="G132" t="n">
         <v>34804196</v>
@@ -3506,7 +3506,7 @@
         <v>1769.390380859375</v>
       </c>
       <c r="F133" t="n">
-        <v>1745.398559570312</v>
+        <v>1745.398681640625</v>
       </c>
       <c r="G133" t="n">
         <v>33665564</v>
@@ -3529,7 +3529,7 @@
         <v>1702.011352539062</v>
       </c>
       <c r="F134" t="n">
-        <v>1678.933349609375</v>
+        <v>1678.933227539062</v>
       </c>
       <c r="G134" t="n">
         <v>69834886</v>
@@ -3575,7 +3575,7 @@
         <v>1764.49853515625</v>
       </c>
       <c r="F136" t="n">
-        <v>1740.573120117188</v>
+        <v>1740.5732421875</v>
       </c>
       <c r="G136" t="n">
         <v>24863382</v>
@@ -3667,7 +3667,7 @@
         <v>1899.348754882812</v>
       </c>
       <c r="F140" t="n">
-        <v>1873.594970703125</v>
+        <v>1873.594848632812</v>
       </c>
       <c r="G140" t="n">
         <v>29166875</v>
@@ -3690,7 +3690,7 @@
         <v>1980.895751953125</v>
       </c>
       <c r="F141" t="n">
-        <v>1954.0361328125</v>
+        <v>1954.036010742188</v>
       </c>
       <c r="G141" t="n">
         <v>60298686</v>
@@ -3782,7 +3782,7 @@
         <v>1946.467895507812</v>
       </c>
       <c r="F145" t="n">
-        <v>1920.0751953125</v>
+        <v>1920.075073242188</v>
       </c>
       <c r="G145" t="n">
         <v>36428722</v>
@@ -3828,7 +3828,7 @@
         <v>1854.306396484375</v>
       </c>
       <c r="F147" t="n">
-        <v>1829.163330078125</v>
+        <v>1829.163208007812</v>
       </c>
       <c r="G147" t="n">
         <v>23357691</v>
@@ -3897,7 +3897,7 @@
         <v>1969.773559570312</v>
       </c>
       <c r="F150" t="n">
-        <v>1943.064819335938</v>
+        <v>1943.06494140625</v>
       </c>
       <c r="G150" t="n">
         <v>24661487</v>
@@ -3920,7 +3920,7 @@
         <v>1981.172607421875</v>
       </c>
       <c r="F151" t="n">
-        <v>1954.309204101562</v>
+        <v>1954.309326171875</v>
       </c>
       <c r="G151" t="n">
         <v>16492208</v>
@@ -3943,7 +3943,7 @@
         <v>1956.620849609375</v>
       </c>
       <c r="F152" t="n">
-        <v>1930.090454101562</v>
+        <v>1930.09033203125</v>
       </c>
       <c r="G152" t="n">
         <v>13479498</v>
@@ -4035,7 +4035,7 @@
         <v>1951.036743164062</v>
       </c>
       <c r="F156" t="n">
-        <v>1924.582153320312</v>
+        <v>1924.58203125</v>
       </c>
       <c r="G156" t="n">
         <v>16612317</v>
@@ -4058,7 +4058,7 @@
         <v>1930.3154296875</v>
       </c>
       <c r="F157" t="n">
-        <v>1904.141723632812</v>
+        <v>1904.1416015625</v>
       </c>
       <c r="G157" t="n">
         <v>15489533</v>
@@ -4081,7 +4081,7 @@
         <v>1955.421020507812</v>
       </c>
       <c r="F158" t="n">
-        <v>1928.906982421875</v>
+        <v>1928.906860351562</v>
       </c>
       <c r="G158" t="n">
         <v>15273836</v>
@@ -4127,7 +4127,7 @@
         <v>1935.576416015625</v>
       </c>
       <c r="F160" t="n">
-        <v>1909.331420898438</v>
+        <v>1909.331298828125</v>
       </c>
       <c r="G160" t="n">
         <v>11268922</v>
@@ -4173,7 +4173,7 @@
         <v>1934.376586914062</v>
       </c>
       <c r="F162" t="n">
-        <v>1908.147827148438</v>
+        <v>1908.147583007812</v>
       </c>
       <c r="G162" t="n">
         <v>16358609</v>
@@ -4196,7 +4196,7 @@
         <v>1921.777587890625</v>
       </c>
       <c r="F163" t="n">
-        <v>1895.719604492188</v>
+        <v>1895.7197265625</v>
       </c>
       <c r="G163" t="n">
         <v>9694004</v>
@@ -4242,7 +4242,7 @@
         <v>1948.083129882812</v>
       </c>
       <c r="F165" t="n">
-        <v>1921.668579101562</v>
+        <v>1921.66845703125</v>
       </c>
       <c r="G165" t="n">
         <v>14042531</v>
@@ -4265,7 +4265,7 @@
         <v>1953.205810546875</v>
       </c>
       <c r="F166" t="n">
-        <v>1926.721801757812</v>
+        <v>1926.7216796875</v>
       </c>
       <c r="G166" t="n">
         <v>13583450</v>
@@ -4334,7 +4334,7 @@
         <v>1964.327880859375</v>
       </c>
       <c r="F169" t="n">
-        <v>1937.69287109375</v>
+        <v>1937.692993164062</v>
       </c>
       <c r="G169" t="n">
         <v>13474719</v>
@@ -4357,7 +4357,7 @@
         <v>1949.467651367188</v>
       </c>
       <c r="F170" t="n">
-        <v>1923.0341796875</v>
+        <v>1923.034301757812</v>
       </c>
       <c r="G170" t="n">
         <v>9293214</v>
@@ -4380,7 +4380,7 @@
         <v>1917.301025390625</v>
       </c>
       <c r="F171" t="n">
-        <v>1891.3037109375</v>
+        <v>1891.303833007812</v>
       </c>
       <c r="G171" t="n">
         <v>14237972</v>
@@ -4403,7 +4403,7 @@
         <v>1922.285278320312</v>
       </c>
       <c r="F172" t="n">
-        <v>1896.220581054688</v>
+        <v>1896.220336914062</v>
       </c>
       <c r="G172" t="n">
         <v>10963236</v>
@@ -4426,7 +4426,7 @@
         <v>1944.852661132812</v>
       </c>
       <c r="F173" t="n">
-        <v>1918.481811523438</v>
+        <v>1918.481689453125</v>
       </c>
       <c r="G173" t="n">
         <v>13698541</v>
@@ -4610,7 +4610,7 @@
         <v>2128.160400390625</v>
       </c>
       <c r="F181" t="n">
-        <v>2099.3037109375</v>
+        <v>2099.303955078125</v>
       </c>
       <c r="G181" t="n">
         <v>16537457</v>
@@ -4633,7 +4633,7 @@
         <v>2082.14892578125</v>
       </c>
       <c r="F182" t="n">
-        <v>2053.91650390625</v>
+        <v>2053.916259765625</v>
       </c>
       <c r="G182" t="n">
         <v>16813690</v>
@@ -4679,7 +4679,7 @@
         <v>2059.027587890625</v>
       </c>
       <c r="F184" t="n">
-        <v>2031.108520507812</v>
+        <v>2031.108642578125</v>
       </c>
       <c r="G184" t="n">
         <v>21494354</v>
@@ -4702,7 +4702,7 @@
         <v>2013.246948242188</v>
       </c>
       <c r="F185" t="n">
-        <v>1985.948852539062</v>
+        <v>1985.94873046875</v>
       </c>
       <c r="G185" t="n">
         <v>14913159</v>
@@ -4748,7 +4748,7 @@
         <v>2045.598022460938</v>
       </c>
       <c r="F187" t="n">
-        <v>2017.861083984375</v>
+        <v>2017.861206054688</v>
       </c>
       <c r="G187" t="n">
         <v>9833424</v>
@@ -4771,7 +4771,7 @@
         <v>2072.180419921875</v>
       </c>
       <c r="F188" t="n">
-        <v>2044.083129882812</v>
+        <v>2044.082885742188</v>
       </c>
       <c r="G188" t="n">
         <v>12921269</v>
@@ -4794,7 +4794,7 @@
         <v>2062.304443359375</v>
       </c>
       <c r="F189" t="n">
-        <v>2034.341064453125</v>
+        <v>2034.340942382812</v>
       </c>
       <c r="G189" t="n">
         <v>12232579</v>
@@ -4817,7 +4817,7 @@
         <v>2053.905029296875</v>
       </c>
       <c r="F190" t="n">
-        <v>2026.055541992188</v>
+        <v>2026.055419921875</v>
       </c>
       <c r="G190" t="n">
         <v>10391613</v>
@@ -4909,7 +4909,7 @@
         <v>2066.826904296875</v>
       </c>
       <c r="F194" t="n">
-        <v>2038.802124023438</v>
+        <v>2038.80224609375</v>
       </c>
       <c r="G194" t="n">
         <v>10538904</v>
@@ -4932,7 +4932,7 @@
         <v>2061.4736328125</v>
       </c>
       <c r="F195" t="n">
-        <v>2033.521362304688</v>
+        <v>2033.521484375</v>
       </c>
       <c r="G195" t="n">
         <v>9272749</v>
@@ -4955,7 +4955,7 @@
         <v>2064.79638671875</v>
       </c>
       <c r="F196" t="n">
-        <v>2036.799072265625</v>
+        <v>2036.799194335938</v>
       </c>
       <c r="G196" t="n">
         <v>7113236</v>
@@ -4978,7 +4978,7 @@
         <v>2105.08544921875</v>
       </c>
       <c r="F197" t="n">
-        <v>2076.542236328125</v>
+        <v>2076.5419921875</v>
       </c>
       <c r="G197" t="n">
         <v>11556006</v>
@@ -5024,7 +5024,7 @@
         <v>2036.598754882812</v>
       </c>
       <c r="F199" t="n">
-        <v>2008.98388671875</v>
+        <v>2008.983764648438</v>
       </c>
       <c r="G199" t="n">
         <v>10018098</v>
@@ -5070,7 +5070,7 @@
         <v>2008.6318359375</v>
       </c>
       <c r="F201" t="n">
-        <v>1981.396118164062</v>
+        <v>1981.396240234375</v>
       </c>
       <c r="G201" t="n">
         <v>15600192</v>
@@ -5208,7 +5208,7 @@
         <v>1877.842895507812</v>
       </c>
       <c r="F207" t="n">
-        <v>1852.380737304688</v>
+        <v>1852.380615234375</v>
       </c>
       <c r="G207" t="n">
         <v>18239448</v>
@@ -5231,7 +5231,7 @@
         <v>1856.567749023438</v>
       </c>
       <c r="F208" t="n">
-        <v>1831.39404296875</v>
+        <v>1831.393798828125</v>
       </c>
       <c r="G208" t="n">
         <v>14962008</v>
@@ -5277,7 +5277,7 @@
         <v>1896.302856445312</v>
       </c>
       <c r="F210" t="n">
-        <v>1870.59033203125</v>
+        <v>1870.590209960938</v>
       </c>
       <c r="G210" t="n">
         <v>17010781</v>
@@ -5323,7 +5323,7 @@
         <v>1707.918579101562</v>
       </c>
       <c r="F212" t="n">
-        <v>1684.760498046875</v>
+        <v>1684.760375976562</v>
       </c>
       <c r="G212" t="n">
         <v>44345811</v>
@@ -5346,7 +5346,7 @@
         <v>1765.882934570312</v>
       </c>
       <c r="F213" t="n">
-        <v>1741.938842773438</v>
+        <v>1741.938720703125</v>
       </c>
       <c r="G213" t="n">
         <v>40090058</v>
@@ -5461,7 +5461,7 @@
         <v>1843.414916992188</v>
       </c>
       <c r="F218" t="n">
-        <v>1818.419311523438</v>
+        <v>1818.419555664062</v>
       </c>
       <c r="G218" t="n">
         <v>28362390</v>
@@ -5530,7 +5530,7 @@
         <v>1848.122192382812</v>
       </c>
       <c r="F221" t="n">
-        <v>1823.062866210938</v>
+        <v>1823.063110351562</v>
       </c>
       <c r="G221" t="n">
         <v>2613110</v>
@@ -5599,7 +5599,7 @@
         <v>1821.216796875</v>
       </c>
       <c r="F224" t="n">
-        <v>1796.522338867188</v>
+        <v>1796.5224609375</v>
       </c>
       <c r="G224" t="n">
         <v>13898171</v>
@@ -5645,7 +5645,7 @@
         <v>1800.495483398438</v>
       </c>
       <c r="F226" t="n">
-        <v>1776.08203125</v>
+        <v>1776.081909179688</v>
       </c>
       <c r="G226" t="n">
         <v>22663783</v>
@@ -5714,7 +5714,7 @@
         <v>1802.249145507812</v>
       </c>
       <c r="F229" t="n">
-        <v>1777.811889648438</v>
+        <v>1777.81201171875</v>
       </c>
       <c r="G229" t="n">
         <v>12919318</v>
@@ -5783,7 +5783,7 @@
         <v>1807.371826171875</v>
       </c>
       <c r="F232" t="n">
-        <v>1782.865112304688</v>
+        <v>1782.865234375</v>
       </c>
       <c r="G232" t="n">
         <v>11094443</v>
@@ -5829,7 +5829,7 @@
         <v>1796.849609375</v>
       </c>
       <c r="F234" t="n">
-        <v>1772.485595703125</v>
+        <v>1772.485473632812</v>
       </c>
       <c r="G234" t="n">
         <v>9232276</v>
@@ -5875,7 +5875,7 @@
         <v>1840.230590820312</v>
       </c>
       <c r="F236" t="n">
-        <v>1815.278198242188</v>
+        <v>1815.2783203125</v>
       </c>
       <c r="G236" t="n">
         <v>21701530</v>
@@ -5898,7 +5898,7 @@
         <v>1870.874145507812</v>
       </c>
       <c r="F237" t="n">
-        <v>1845.50634765625</v>
+        <v>1845.506469726562</v>
       </c>
       <c r="G237" t="n">
         <v>14587627</v>
@@ -5921,7 +5921,7 @@
         <v>1852.460327148438</v>
       </c>
       <c r="F238" t="n">
-        <v>1827.34228515625</v>
+        <v>1827.342163085938</v>
       </c>
       <c r="G238" t="n">
         <v>8032753</v>
@@ -6036,7 +6036,7 @@
         <v>1832.708129882812</v>
       </c>
       <c r="F243" t="n">
-        <v>1807.85791015625</v>
+        <v>1807.858032226562</v>
       </c>
       <c r="G243" t="n">
         <v>10126179</v>
@@ -6059,7 +6059,7 @@
         <v>1838.199951171875</v>
       </c>
       <c r="F244" t="n">
-        <v>1813.275268554688</v>
+        <v>1813.275146484375</v>
       </c>
       <c r="G244" t="n">
         <v>9233172</v>
@@ -6151,7 +6151,7 @@
         <v>1840.599853515625</v>
       </c>
       <c r="F248" t="n">
-        <v>1815.642700195312</v>
+        <v>1815.642578125</v>
       </c>
       <c r="G248" t="n">
         <v>10388494</v>
@@ -6197,7 +6197,7 @@
         <v>1836.815551757812</v>
       </c>
       <c r="F250" t="n">
-        <v>1811.909545898438</v>
+        <v>1811.90966796875</v>
       </c>
       <c r="G250" t="n">
         <v>9305969</v>
@@ -6220,7 +6220,7 @@
         <v>1841.845825195312</v>
       </c>
       <c r="F251" t="n">
-        <v>1816.871704101562</v>
+        <v>1816.87158203125</v>
       </c>
       <c r="G251" t="n">
         <v>11021815</v>
@@ -6243,7 +6243,7 @@
         <v>1832.431274414062</v>
       </c>
       <c r="F252" t="n">
-        <v>1807.584838867188</v>
+        <v>1807.584716796875</v>
       </c>
       <c r="G252" t="n">
         <v>9390594</v>
@@ -6312,7 +6312,7 @@
         <v>1814.709716796875</v>
       </c>
       <c r="F255" t="n">
-        <v>1790.103393554688</v>
+        <v>1790.103515625</v>
       </c>
       <c r="G255" t="n">
         <v>12061545</v>
@@ -6335,7 +6335,7 @@
         <v>1766.852172851562</v>
       </c>
       <c r="F256" t="n">
-        <v>1742.894897460938</v>
+        <v>1742.894775390625</v>
       </c>
       <c r="G256" t="n">
         <v>23200734</v>
@@ -6358,7 +6358,7 @@
         <v>1763.990844726562</v>
       </c>
       <c r="F257" t="n">
-        <v>1740.072387695312</v>
+        <v>1740.072265625</v>
       </c>
       <c r="G257" t="n">
         <v>16162959</v>
@@ -6381,7 +6381,7 @@
         <v>1784.804443359375</v>
       </c>
       <c r="F258" t="n">
-        <v>1760.603881835938</v>
+        <v>1760.603759765625</v>
       </c>
       <c r="G258" t="n">
         <v>13770093</v>
@@ -6404,7 +6404,7 @@
         <v>1751.1611328125</v>
       </c>
       <c r="F259" t="n">
-        <v>1727.416625976562</v>
+        <v>1727.41650390625</v>
       </c>
       <c r="G259" t="n">
         <v>16653912</v>
@@ -6427,7 +6427,7 @@
         <v>1806.356567382812</v>
       </c>
       <c r="F260" t="n">
-        <v>1781.863647460938</v>
+        <v>1781.86376953125</v>
       </c>
       <c r="G260" t="n">
         <v>20580773</v>
@@ -6588,7 +6588,7 @@
         <v>1937.745483398438</v>
       </c>
       <c r="F267" t="n">
-        <v>1911.471069335938</v>
+        <v>1911.470947265625</v>
       </c>
       <c r="G267" t="n">
         <v>19543871</v>
@@ -6634,7 +6634,7 @@
         <v>1791.542358398438</v>
       </c>
       <c r="F269" t="n">
-        <v>1767.250366210938</v>
+        <v>1767.250244140625</v>
       </c>
       <c r="G269" t="n">
         <v>27103552</v>
@@ -6657,7 +6657,7 @@
         <v>1749.084350585938</v>
       </c>
       <c r="F270" t="n">
-        <v>1725.367919921875</v>
+        <v>1725.368041992188</v>
       </c>
       <c r="G270" t="n">
         <v>21185065</v>
@@ -6680,7 +6680,7 @@
         <v>1732.055053710938</v>
       </c>
       <c r="F271" t="n">
-        <v>1708.569458007812</v>
+        <v>1708.569580078125</v>
       </c>
       <c r="G271" t="n">
         <v>17033907</v>
@@ -6749,7 +6749,7 @@
         <v>1777.512817382812</v>
       </c>
       <c r="F274" t="n">
-        <v>1753.411010742188</v>
+        <v>1753.410888671875</v>
       </c>
       <c r="G274" t="n">
         <v>20735017</v>
@@ -6795,7 +6795,7 @@
         <v>1776.128295898438</v>
       </c>
       <c r="F276" t="n">
-        <v>1752.045043945312</v>
+        <v>1752.045166015625</v>
       </c>
       <c r="G276" t="n">
         <v>12813490</v>
@@ -6864,7 +6864,7 @@
         <v>1805.525756835938</v>
       </c>
       <c r="F279" t="n">
-        <v>1781.044067382812</v>
+        <v>1781.044189453125</v>
       </c>
       <c r="G279" t="n">
         <v>9802070</v>
@@ -6933,7 +6933,7 @@
         <v>1884.396118164062</v>
       </c>
       <c r="F282" t="n">
-        <v>1858.845092773438</v>
+        <v>1858.844848632812</v>
       </c>
       <c r="G282" t="n">
         <v>15248514</v>
@@ -6956,7 +6956,7 @@
         <v>1876.089111328125</v>
       </c>
       <c r="F283" t="n">
-        <v>1850.650756835938</v>
+        <v>1850.650634765625</v>
       </c>
       <c r="G283" t="n">
         <v>7895549</v>
@@ -7002,7 +7002,7 @@
         <v>1922.839111328125</v>
       </c>
       <c r="F285" t="n">
-        <v>1896.766723632812</v>
+        <v>1896.766845703125</v>
       </c>
       <c r="G285" t="n">
         <v>11871497</v>
@@ -7025,7 +7025,7 @@
         <v>1908.486450195312</v>
       </c>
       <c r="F286" t="n">
-        <v>1882.60888671875</v>
+        <v>1882.608642578125</v>
       </c>
       <c r="G286" t="n">
         <v>9323438</v>
@@ -7117,7 +7117,7 @@
         <v>1902.302368164062</v>
       </c>
       <c r="F290" t="n">
-        <v>1876.508544921875</v>
+        <v>1876.508422851562</v>
       </c>
       <c r="G290" t="n">
         <v>5403831</v>
@@ -7140,7 +7140,7 @@
         <v>1979.234375</v>
       </c>
       <c r="F291" t="n">
-        <v>1952.397338867188</v>
+        <v>1952.397216796875</v>
       </c>
       <c r="G291" t="n">
         <v>17427846</v>
@@ -7163,7 +7163,7 @@
         <v>1925.192749023438</v>
       </c>
       <c r="F292" t="n">
-        <v>1899.08837890625</v>
+        <v>1899.088500976562</v>
       </c>
       <c r="G292" t="n">
         <v>18740607</v>
@@ -7186,7 +7186,7 @@
         <v>1939.868408203125</v>
       </c>
       <c r="F293" t="n">
-        <v>1913.565063476562</v>
+        <v>1913.565185546875</v>
       </c>
       <c r="G293" t="n">
         <v>8840382</v>
@@ -7232,7 +7232,7 @@
         <v>2032.53759765625</v>
       </c>
       <c r="F295" t="n">
-        <v>2004.977783203125</v>
+        <v>2004.977661132812</v>
       </c>
       <c r="G295" t="n">
         <v>15962230</v>
@@ -7255,7 +7255,7 @@
         <v>2008.308837890625</v>
       </c>
       <c r="F296" t="n">
-        <v>1981.07763671875</v>
+        <v>1981.077514648438</v>
       </c>
       <c r="G296" t="n">
         <v>10717877</v>
@@ -7393,7 +7393,7 @@
         <v>1946.514038085938</v>
       </c>
       <c r="F302" t="n">
-        <v>1920.120727539062</v>
+        <v>1920.12060546875</v>
       </c>
       <c r="G302" t="n">
         <v>8349049</v>
@@ -7416,7 +7416,7 @@
         <v>1938.853149414062</v>
       </c>
       <c r="F303" t="n">
-        <v>1912.563598632812</v>
+        <v>1912.563720703125</v>
       </c>
       <c r="G303" t="n">
         <v>6936900</v>
@@ -7439,7 +7439,7 @@
         <v>1897.08740234375</v>
       </c>
       <c r="F304" t="n">
-        <v>1871.364135742188</v>
+        <v>1871.364379882812</v>
       </c>
       <c r="G304" t="n">
         <v>9605118</v>
@@ -7462,7 +7462,7 @@
         <v>1854.398681640625</v>
       </c>
       <c r="F305" t="n">
-        <v>1829.25439453125</v>
+        <v>1829.254272460938</v>
       </c>
       <c r="G305" t="n">
         <v>10323740</v>
@@ -7485,7 +7485,7 @@
         <v>1921.685302734375</v>
       </c>
       <c r="F306" t="n">
-        <v>1895.628662109375</v>
+        <v>1895.628540039062</v>
       </c>
       <c r="G306" t="n">
         <v>20893714</v>
@@ -7508,7 +7508,7 @@
         <v>1903.594482421875</v>
       </c>
       <c r="F307" t="n">
-        <v>1877.783203125</v>
+        <v>1877.783081054688</v>
       </c>
       <c r="G307" t="n">
         <v>9286239</v>
@@ -7531,7 +7531,7 @@
         <v>1926.761840820312</v>
       </c>
       <c r="F308" t="n">
-        <v>1900.63623046875</v>
+        <v>1900.636352539062</v>
       </c>
       <c r="G308" t="n">
         <v>8710582</v>
@@ -7554,7 +7554,7 @@
         <v>1889.6572265625</v>
       </c>
       <c r="F309" t="n">
-        <v>1864.034790039062</v>
+        <v>1864.034912109375</v>
       </c>
       <c r="G309" t="n">
         <v>8411407</v>
@@ -7600,7 +7600,7 @@
         <v>1841.061279296875</v>
       </c>
       <c r="F311" t="n">
-        <v>1816.09765625</v>
+        <v>1816.097778320312</v>
       </c>
       <c r="G311" t="n">
         <v>10090101</v>
@@ -7715,7 +7715,7 @@
         <v>1831.50830078125</v>
       </c>
       <c r="F316" t="n">
-        <v>1806.674194335938</v>
+        <v>1806.674438476562</v>
       </c>
       <c r="G316" t="n">
         <v>7004597</v>
@@ -7784,7 +7784,7 @@
         <v>1829.431518554688</v>
       </c>
       <c r="F319" t="n">
-        <v>1804.625732421875</v>
+        <v>1804.625610351562</v>
       </c>
       <c r="G319" t="n">
         <v>7018942</v>
@@ -7807,7 +7807,7 @@
         <v>1763.990844726562</v>
       </c>
       <c r="F320" t="n">
-        <v>1740.072387695312</v>
+        <v>1740.072265625</v>
       </c>
       <c r="G320" t="n">
         <v>10450741</v>
@@ -7830,7 +7830,7 @@
         <v>1783.05078125</v>
       </c>
       <c r="F321" t="n">
-        <v>1758.873779296875</v>
+        <v>1758.873901367188</v>
       </c>
       <c r="G321" t="n">
         <v>9705594</v>
@@ -7853,7 +7853,7 @@
         <v>1794.588256835938</v>
       </c>
       <c r="F322" t="n">
-        <v>1770.255004882812</v>
+        <v>1770.2548828125</v>
       </c>
       <c r="G322" t="n">
         <v>9861858</v>
@@ -7876,7 +7876,7 @@
         <v>1783.32763671875</v>
       </c>
       <c r="F323" t="n">
-        <v>1759.147094726562</v>
+        <v>1759.14697265625</v>
       </c>
       <c r="G323" t="n">
         <v>7828474</v>
@@ -7945,7 +7945,7 @@
         <v>1759.606567382812</v>
       </c>
       <c r="F326" t="n">
-        <v>1735.74755859375</v>
+        <v>1735.747436523438</v>
       </c>
       <c r="G326" t="n">
         <v>7245477</v>
@@ -7968,7 +7968,7 @@
         <v>1757.714477539062</v>
       </c>
       <c r="F327" t="n">
-        <v>1733.881225585938</v>
+        <v>1733.881103515625</v>
       </c>
       <c r="G327" t="n">
         <v>5914428</v>
@@ -8014,7 +8014,7 @@
         <v>1835.523315429688</v>
       </c>
       <c r="F329" t="n">
-        <v>1810.634765625</v>
+        <v>1810.634887695312</v>
       </c>
       <c r="G329" t="n">
         <v>9996262</v>
@@ -8037,7 +8037,7 @@
         <v>1843.507202148438</v>
       </c>
       <c r="F330" t="n">
-        <v>1818.510620117188</v>
+        <v>1818.510375976562</v>
       </c>
       <c r="G330" t="n">
         <v>8561218</v>
@@ -8106,7 +8106,7 @@
         <v>1808.202514648438</v>
       </c>
       <c r="F333" t="n">
-        <v>1783.684692382812</v>
+        <v>1783.6845703125</v>
       </c>
       <c r="G333" t="n">
         <v>11820093</v>
@@ -8129,7 +8129,7 @@
         <v>1769.021118164062</v>
       </c>
       <c r="F334" t="n">
-        <v>1745.034545898438</v>
+        <v>1745.034423828125</v>
       </c>
       <c r="G334" t="n">
         <v>10924915</v>
@@ -8221,7 +8221,7 @@
         <v>1777.881958007812</v>
       </c>
       <c r="F338" t="n">
-        <v>1753.775146484375</v>
+        <v>1753.775268554688</v>
       </c>
       <c r="G338" t="n">
         <v>6970618</v>
@@ -8244,7 +8244,7 @@
         <v>1784.296875</v>
       </c>
       <c r="F339" t="n">
-        <v>1760.10302734375</v>
+        <v>1760.102905273438</v>
       </c>
       <c r="G339" t="n">
         <v>6739132</v>
@@ -8267,7 +8267,7 @@
         <v>1765.836791992188</v>
       </c>
       <c r="F340" t="n">
-        <v>1741.893310546875</v>
+        <v>1741.893188476562</v>
       </c>
       <c r="G340" t="n">
         <v>6588980</v>
@@ -8313,7 +8313,7 @@
         <v>1809.402465820312</v>
       </c>
       <c r="F342" t="n">
-        <v>1784.8681640625</v>
+        <v>1784.868286132812</v>
       </c>
       <c r="G342" t="n">
         <v>5936539</v>
@@ -8336,7 +8336,7 @@
         <v>1834.877197265625</v>
       </c>
       <c r="F343" t="n">
-        <v>1809.997436523438</v>
+        <v>1809.99755859375</v>
       </c>
       <c r="G343" t="n">
         <v>6032459</v>
@@ -8359,7 +8359,7 @@
         <v>1843.276489257812</v>
       </c>
       <c r="F344" t="n">
-        <v>1818.282836914062</v>
+        <v>1818.282958984375</v>
       </c>
       <c r="G344" t="n">
         <v>8158501</v>
@@ -8382,7 +8382,7 @@
         <v>1832.523559570312</v>
       </c>
       <c r="F345" t="n">
-        <v>1807.675659179688</v>
+        <v>1807.675903320312</v>
       </c>
       <c r="G345" t="n">
         <v>5711266</v>
@@ -8405,7 +8405,7 @@
         <v>1848.35302734375</v>
       </c>
       <c r="F346" t="n">
-        <v>1823.290649414062</v>
+        <v>1823.29052734375</v>
       </c>
       <c r="G346" t="n">
         <v>5392802</v>
@@ -8428,7 +8428,7 @@
         <v>1832.754272460938</v>
       </c>
       <c r="F347" t="n">
-        <v>1807.903442382812</v>
+        <v>1807.9033203125</v>
       </c>
       <c r="G347" t="n">
         <v>4275880</v>
@@ -8451,7 +8451,7 @@
         <v>1811.98681640625</v>
       </c>
       <c r="F348" t="n">
-        <v>1787.41748046875</v>
+        <v>1787.417602539062</v>
       </c>
       <c r="G348" t="n">
         <v>7390051</v>
@@ -8474,7 +8474,7 @@
         <v>1818.35546875</v>
       </c>
       <c r="F349" t="n">
-        <v>1793.699829101562</v>
+        <v>1793.69970703125</v>
       </c>
       <c r="G349" t="n">
         <v>3740102</v>
@@ -8497,7 +8497,7 @@
         <v>1823.939697265625</v>
       </c>
       <c r="F350" t="n">
-        <v>1799.208374023438</v>
+        <v>1799.20849609375</v>
       </c>
       <c r="G350" t="n">
         <v>13409647</v>
@@ -8543,7 +8543,7 @@
         <v>1993.956176757812</v>
       </c>
       <c r="F352" t="n">
-        <v>1966.91943359375</v>
+        <v>1966.919555664062</v>
       </c>
       <c r="G352" t="n">
         <v>29562071</v>
@@ -8566,7 +8566,7 @@
         <v>2001.89404296875</v>
       </c>
       <c r="F353" t="n">
-        <v>1974.749755859375</v>
+        <v>1974.749877929688</v>
       </c>
       <c r="G353" t="n">
         <v>14006916</v>
@@ -8589,7 +8589,7 @@
         <v>2031.753051757812</v>
       </c>
       <c r="F354" t="n">
-        <v>2004.203979492188</v>
+        <v>2004.203857421875</v>
       </c>
       <c r="G354" t="n">
         <v>12315081</v>
@@ -8612,7 +8612,7 @@
         <v>2039.506225585938</v>
       </c>
       <c r="F355" t="n">
-        <v>2011.851928710938</v>
+        <v>2011.851806640625</v>
       </c>
       <c r="G355" t="n">
         <v>11987128</v>
@@ -8635,7 +8635,7 @@
         <v>2021.830810546875</v>
       </c>
       <c r="F356" t="n">
-        <v>1994.416259765625</v>
+        <v>1994.416137695312</v>
       </c>
       <c r="G356" t="n">
         <v>7234323</v>
@@ -8681,7 +8681,7 @@
         <v>2044.075073242188</v>
       </c>
       <c r="F358" t="n">
-        <v>2016.359008789062</v>
+        <v>2016.35888671875</v>
       </c>
       <c r="G358" t="n">
         <v>4837367</v>
@@ -8934,7 +8934,7 @@
         <v>2035.537353515625</v>
       </c>
       <c r="F369" t="n">
-        <v>2014.93701171875</v>
+        <v>2014.936889648438</v>
       </c>
       <c r="G369" t="n">
         <v>8326975</v>
@@ -9072,7 +9072,7 @@
         <v>1936.4072265625</v>
       </c>
       <c r="F375" t="n">
-        <v>1916.81005859375</v>
+        <v>1916.810180664062</v>
       </c>
       <c r="G375" t="n">
         <v>6267203</v>
@@ -9095,7 +9095,7 @@
         <v>1965.112426757812</v>
       </c>
       <c r="F376" t="n">
-        <v>1945.224853515625</v>
+        <v>1945.224731445312</v>
       </c>
       <c r="G376" t="n">
         <v>7043310</v>
@@ -9118,7 +9118,7 @@
         <v>1984.633911132812</v>
       </c>
       <c r="F377" t="n">
-        <v>1964.548828125</v>
+        <v>1964.548706054688</v>
       </c>
       <c r="G377" t="n">
         <v>5851143</v>
@@ -9371,7 +9371,7 @@
         <v>1932.57666015625</v>
       </c>
       <c r="F388" t="n">
-        <v>1913.018310546875</v>
+        <v>1913.018188476562</v>
       </c>
       <c r="G388" t="n">
         <v>3370732</v>
@@ -9417,7 +9417,7 @@
         <v>1943.560424804688</v>
       </c>
       <c r="F390" t="n">
-        <v>1923.890869140625</v>
+        <v>1923.890991210938</v>
       </c>
       <c r="G390" t="n">
         <v>4968515</v>
@@ -9440,7 +9440,7 @@
         <v>1916.931884765625</v>
       </c>
       <c r="F391" t="n">
-        <v>1897.531860351562</v>
+        <v>1897.531982421875</v>
       </c>
       <c r="G391" t="n">
         <v>6194834</v>
@@ -9486,7 +9486,7 @@
         <v>1880.473388671875</v>
       </c>
       <c r="F393" t="n">
-        <v>1861.442260742188</v>
+        <v>1861.4423828125</v>
       </c>
       <c r="G393" t="n">
         <v>6448924</v>
@@ -9509,7 +9509,7 @@
         <v>1895.149047851562</v>
       </c>
       <c r="F394" t="n">
-        <v>1875.969360351562</v>
+        <v>1875.969482421875</v>
       </c>
       <c r="G394" t="n">
         <v>6882869</v>
@@ -9578,7 +9578,7 @@
         <v>1926.992553710938</v>
       </c>
       <c r="F397" t="n">
-        <v>1907.49072265625</v>
+        <v>1907.490600585938</v>
       </c>
       <c r="G397" t="n">
         <v>5908649</v>
@@ -9601,7 +9601,7 @@
         <v>1941.760620117188</v>
       </c>
       <c r="F398" t="n">
-        <v>1922.109375</v>
+        <v>1922.109252929688</v>
       </c>
       <c r="G398" t="n">
         <v>6584900</v>
@@ -9670,7 +9670,7 @@
         <v>1917.208740234375</v>
       </c>
       <c r="F401" t="n">
-        <v>1897.805786132812</v>
+        <v>1897.805908203125</v>
       </c>
       <c r="G401" t="n">
         <v>3747071</v>
@@ -9762,7 +9762,7 @@
         <v>1980.434204101562</v>
       </c>
       <c r="F405" t="n">
-        <v>1960.391479492188</v>
+        <v>1960.3916015625</v>
       </c>
       <c r="G405" t="n">
         <v>6390450</v>
@@ -9785,7 +9785,7 @@
         <v>2006.139770507812</v>
       </c>
       <c r="F406" t="n">
-        <v>1985.837036132812</v>
+        <v>1985.8369140625</v>
       </c>
       <c r="G406" t="n">
         <v>10967722</v>
@@ -9808,7 +9808,7 @@
         <v>1997.60205078125</v>
       </c>
       <c r="F407" t="n">
-        <v>1977.385620117188</v>
+        <v>1977.3857421875</v>
       </c>
       <c r="G407" t="n">
         <v>6329084</v>
@@ -9831,7 +9831,7 @@
         <v>2005.355224609375</v>
       </c>
       <c r="F408" t="n">
-        <v>1985.060302734375</v>
+        <v>1985.060424804688</v>
       </c>
       <c r="G408" t="n">
         <v>5037930</v>
@@ -9877,7 +9877,7 @@
         <v>1995.848388671875</v>
       </c>
       <c r="F410" t="n">
-        <v>1975.649780273438</v>
+        <v>1975.649658203125</v>
       </c>
       <c r="G410" t="n">
         <v>4927197</v>
@@ -9900,7 +9900,7 @@
         <v>2015.554443359375</v>
       </c>
       <c r="F411" t="n">
-        <v>1995.15625</v>
+        <v>1995.156372070312</v>
       </c>
       <c r="G411" t="n">
         <v>5932236</v>
@@ -10084,7 +10084,7 @@
         <v>2204.584716796875</v>
       </c>
       <c r="F419" t="n">
-        <v>2182.273681640625</v>
+        <v>2182.2734375</v>
       </c>
       <c r="G419" t="n">
         <v>15332214</v>
@@ -10107,7 +10107,7 @@
         <v>2238.828125</v>
       </c>
       <c r="F420" t="n">
-        <v>2216.170654296875</v>
+        <v>2216.17041015625</v>
       </c>
       <c r="G420" t="n">
         <v>16820855</v>
@@ -10130,7 +10130,7 @@
         <v>2252.949951171875</v>
       </c>
       <c r="F421" t="n">
-        <v>2230.1494140625</v>
+        <v>2230.149169921875</v>
       </c>
       <c r="G421" t="n">
         <v>8674941</v>
@@ -10153,7 +10153,7 @@
         <v>2244.13525390625</v>
       </c>
       <c r="F422" t="n">
-        <v>2221.423828125</v>
+        <v>2221.423583984375</v>
       </c>
       <c r="G422" t="n">
         <v>7150825</v>
@@ -10176,7 +10176,7 @@
         <v>2238.828125</v>
       </c>
       <c r="F423" t="n">
-        <v>2216.170654296875</v>
+        <v>2216.17041015625</v>
       </c>
       <c r="G423" t="n">
         <v>4481624</v>
@@ -10314,7 +10314,7 @@
         <v>2209.984375</v>
       </c>
       <c r="F429" t="n">
-        <v>2187.618408203125</v>
+        <v>2187.61865234375</v>
       </c>
       <c r="G429" t="n">
         <v>5889909</v>
@@ -10498,7 +10498,7 @@
         <v>2325.266845703125</v>
       </c>
       <c r="F437" t="n">
-        <v>2301.734375</v>
+        <v>2301.734130859375</v>
       </c>
       <c r="G437" t="n">
         <v>6795327</v>
@@ -10544,7 +10544,7 @@
         <v>2359.32568359375</v>
       </c>
       <c r="F439" t="n">
-        <v>2335.4482421875</v>
+        <v>2335.448486328125</v>
       </c>
       <c r="G439" t="n">
         <v>5459276</v>
@@ -10567,7 +10567,7 @@
         <v>2408.290771484375</v>
       </c>
       <c r="F440" t="n">
-        <v>2383.918212890625</v>
+        <v>2383.91796875</v>
       </c>
       <c r="G440" t="n">
         <v>6766817</v>
@@ -10590,7 +10590,7 @@
         <v>2362.74072265625</v>
       </c>
       <c r="F441" t="n">
-        <v>2338.828857421875</v>
+        <v>2338.8291015625</v>
       </c>
       <c r="G441" t="n">
         <v>5129440</v>
@@ -10705,7 +10705,7 @@
         <v>2487.43798828125</v>
       </c>
       <c r="F446" t="n">
-        <v>2462.264404296875</v>
+        <v>2462.26416015625</v>
       </c>
       <c r="G446" t="n">
         <v>4979881</v>
@@ -10728,7 +10728,7 @@
         <v>2492.46826171875</v>
       </c>
       <c r="F447" t="n">
-        <v>2467.24365234375</v>
+        <v>2467.243896484375</v>
       </c>
       <c r="G447" t="n">
         <v>4311734</v>
@@ -10797,7 +10797,7 @@
         <v>2492.46826171875</v>
       </c>
       <c r="F450" t="n">
-        <v>2467.24365234375</v>
+        <v>2467.243896484375</v>
       </c>
       <c r="G450" t="n">
         <v>6355285</v>
@@ -10820,7 +10820,7 @@
         <v>2420.566650390625</v>
       </c>
       <c r="F451" t="n">
-        <v>2396.069580078125</v>
+        <v>2396.06982421875</v>
       </c>
       <c r="G451" t="n">
         <v>10415834</v>
@@ -10843,7 +10843,7 @@
         <v>2425.08935546875</v>
       </c>
       <c r="F452" t="n">
-        <v>2400.54638671875</v>
+        <v>2400.546630859375</v>
       </c>
       <c r="G452" t="n">
         <v>5513737</v>
@@ -10912,7 +10912,7 @@
         <v>2425.08935546875</v>
       </c>
       <c r="F455" t="n">
-        <v>2400.54638671875</v>
+        <v>2400.546630859375</v>
       </c>
       <c r="G455" t="n">
         <v>4948149</v>
@@ -10958,7 +10958,7 @@
         <v>2340.9580078125</v>
       </c>
       <c r="F457" t="n">
-        <v>2317.2666015625</v>
+        <v>2317.266845703125</v>
       </c>
       <c r="G457" t="n">
         <v>7116512</v>
@@ -10981,7 +10981,7 @@
         <v>2342.388671875</v>
       </c>
       <c r="F458" t="n">
-        <v>2318.68310546875</v>
+        <v>2318.682861328125</v>
       </c>
       <c r="G458" t="n">
         <v>7740557</v>
@@ -11234,7 +11234,7 @@
         <v>2274.271240234375</v>
       </c>
       <c r="F469" t="n">
-        <v>2251.255126953125</v>
+        <v>2251.2548828125</v>
       </c>
       <c r="G469" t="n">
         <v>5101014</v>
@@ -11326,7 +11326,7 @@
         <v>2170.341552734375</v>
       </c>
       <c r="F473" t="n">
-        <v>2148.376953125</v>
+        <v>2148.376708984375</v>
       </c>
       <c r="G473" t="n">
         <v>8410148</v>
@@ -11418,7 +11418,7 @@
         <v>2220.183349609375</v>
       </c>
       <c r="F477" t="n">
-        <v>2197.71435546875</v>
+        <v>2197.714111328125</v>
       </c>
       <c r="G477" t="n">
         <v>16086149</v>
@@ -11556,7 +11556,7 @@
         <v>2231.905517578125</v>
       </c>
       <c r="F483" t="n">
-        <v>2209.31787109375</v>
+        <v>2209.318115234375</v>
       </c>
       <c r="G483" t="n">
         <v>4372089</v>
@@ -11740,7 +11740,7 @@
         <v>2101.993408203125</v>
       </c>
       <c r="F491" t="n">
-        <v>2080.720458984375</v>
+        <v>2080.72021484375</v>
       </c>
       <c r="G491" t="n">
         <v>7162923</v>
@@ -11878,7 +11878,7 @@
         <v>2213.722412109375</v>
       </c>
       <c r="F497" t="n">
-        <v>2191.31884765625</v>
+        <v>2191.318603515625</v>
       </c>
       <c r="G497" t="n">
         <v>3187306</v>
@@ -12016,7 +12016,7 @@
         <v>2279.43994140625</v>
       </c>
       <c r="F503" t="n">
-        <v>2256.37109375</v>
+        <v>2256.371337890625</v>
       </c>
       <c r="G503" t="n">
         <v>5821906</v>
@@ -12039,7 +12039,7 @@
         <v>2230.4287109375</v>
       </c>
       <c r="F504" t="n">
-        <v>2207.856201171875</v>
+        <v>2207.85595703125</v>
       </c>
       <c r="G504" t="n">
         <v>7223711</v>
@@ -12062,7 +12062,7 @@
         <v>2248.42724609375</v>
       </c>
       <c r="F505" t="n">
-        <v>2225.672607421875</v>
+        <v>2225.67236328125</v>
       </c>
       <c r="G505" t="n">
         <v>6556057</v>
@@ -12085,7 +12085,7 @@
         <v>2250.273193359375</v>
       </c>
       <c r="F506" t="n">
-        <v>2227.49951171875</v>
+        <v>2227.499755859375</v>
       </c>
       <c r="G506" t="n">
         <v>4623365</v>
@@ -12131,7 +12131,7 @@
         <v>2326.974365234375</v>
       </c>
       <c r="F508" t="n">
-        <v>2303.42431640625</v>
+        <v>2303.424560546875</v>
       </c>
       <c r="G508" t="n">
         <v>7400221</v>
@@ -12177,7 +12177,7 @@
         <v>2343.49609375</v>
       </c>
       <c r="F510" t="n">
-        <v>2319.779052734375</v>
+        <v>2319.77880859375</v>
       </c>
       <c r="G510" t="n">
         <v>9965088</v>
@@ -12269,7 +12269,7 @@
         <v>2286.685546875</v>
       </c>
       <c r="F514" t="n">
-        <v>2263.54345703125</v>
+        <v>2263.543701171875</v>
       </c>
       <c r="G514" t="n">
         <v>8247243</v>
@@ -12384,7 +12384,7 @@
         <v>2155.98876953125</v>
       </c>
       <c r="F519" t="n">
-        <v>2134.169189453125</v>
+        <v>2134.16943359375</v>
       </c>
       <c r="G519" t="n">
         <v>7333863</v>
@@ -12453,7 +12453,7 @@
         <v>2200.015869140625</v>
       </c>
       <c r="F522" t="n">
-        <v>2177.7509765625</v>
+        <v>2177.750732421875</v>
       </c>
       <c r="G522" t="n">
         <v>5008845</v>
@@ -12476,7 +12476,7 @@
         <v>2171.58740234375</v>
       </c>
       <c r="F523" t="n">
-        <v>2149.610107421875</v>
+        <v>2149.6103515625</v>
       </c>
       <c r="G523" t="n">
         <v>4786419</v>
@@ -12499,7 +12499,7 @@
         <v>2151.7890625</v>
       </c>
       <c r="F524" t="n">
-        <v>2130.012451171875</v>
+        <v>2130.01220703125</v>
       </c>
       <c r="G524" t="n">
         <v>5530620</v>
@@ -12614,7 +12614,7 @@
         <v>2193.41650390625</v>
       </c>
       <c r="F529" t="n">
-        <v>2171.21826171875</v>
+        <v>2171.218505859375</v>
       </c>
       <c r="G529" t="n">
         <v>7971685</v>
@@ -12637,7 +12637,7 @@
         <v>2158.48095703125</v>
       </c>
       <c r="F530" t="n">
-        <v>2136.63623046875</v>
+        <v>2136.636474609375</v>
       </c>
       <c r="G530" t="n">
         <v>5359816</v>
@@ -12660,7 +12660,7 @@
         <v>2231.76708984375</v>
       </c>
       <c r="F531" t="n">
-        <v>2209.1806640625</v>
+        <v>2209.180908203125</v>
       </c>
       <c r="G531" t="n">
         <v>5606335</v>
@@ -12706,7 +12706,7 @@
         <v>2255.349609375</v>
       </c>
       <c r="F533" t="n">
-        <v>2232.524658203125</v>
+        <v>2232.52490234375</v>
       </c>
       <c r="G533" t="n">
         <v>6426626</v>
@@ -12890,7 +12890,7 @@
         <v>2213.86083984375</v>
       </c>
       <c r="F541" t="n">
-        <v>2191.4560546875</v>
+        <v>2191.455810546875</v>
       </c>
       <c r="G541" t="n">
         <v>10735893</v>
@@ -12959,7 +12959,7 @@
         <v>2067.10400390625</v>
       </c>
       <c r="F544" t="n">
-        <v>2046.184204101562</v>
+        <v>2046.184326171875</v>
       </c>
       <c r="G544" t="n">
         <v>8991655</v>
@@ -13074,7 +13074,7 @@
         <v>2232.59765625</v>
       </c>
       <c r="F549" t="n">
-        <v>2210.0029296875</v>
+        <v>2210.003173828125</v>
       </c>
       <c r="G549" t="n">
         <v>4170339</v>
@@ -13120,7 +13120,7 @@
         <v>2218.291259765625</v>
       </c>
       <c r="F551" t="n">
-        <v>2195.84130859375</v>
+        <v>2195.841552734375</v>
       </c>
       <c r="G551" t="n">
         <v>5574914</v>
@@ -13143,7 +13143,7 @@
         <v>2290.6083984375</v>
       </c>
       <c r="F552" t="n">
-        <v>2267.4267578125</v>
+        <v>2267.426513671875</v>
       </c>
       <c r="G552" t="n">
         <v>10711049</v>
@@ -13166,7 +13166,7 @@
         <v>2277.409423828125</v>
       </c>
       <c r="F553" t="n">
-        <v>2254.361083984375</v>
+        <v>2254.361328125</v>
       </c>
       <c r="G553" t="n">
         <v>5999733</v>
@@ -13212,7 +13212,7 @@
         <v>2343.6806640625</v>
       </c>
       <c r="F555" t="n">
-        <v>2319.961669921875</v>
+        <v>2319.9619140625</v>
       </c>
       <c r="G555" t="n">
         <v>7731093</v>
@@ -13235,7 +13235,7 @@
         <v>2380.093017578125</v>
       </c>
       <c r="F556" t="n">
-        <v>2356.005615234375</v>
+        <v>2356.00537109375</v>
       </c>
       <c r="G556" t="n">
         <v>6584133</v>
@@ -13327,7 +13327,7 @@
         <v>2467.132080078125</v>
       </c>
       <c r="F560" t="n">
-        <v>2442.163818359375</v>
+        <v>2442.1640625</v>
       </c>
       <c r="G560" t="n">
         <v>7905775</v>
@@ -13373,7 +13373,7 @@
         <v>2451.3486328125</v>
       </c>
       <c r="F562" t="n">
-        <v>2426.5400390625</v>
+        <v>2426.540283203125</v>
       </c>
       <c r="G562" t="n">
         <v>3961440</v>
@@ -13419,7 +13419,7 @@
         <v>2423.84326171875</v>
       </c>
       <c r="F564" t="n">
-        <v>2399.31298828125</v>
+        <v>2399.313232421875</v>
       </c>
       <c r="G564" t="n">
         <v>6574935</v>
@@ -13580,7 +13580,7 @@
         <v>2347.97265625</v>
       </c>
       <c r="F571" t="n">
-        <v>2324.21044921875</v>
+        <v>2324.210205078125</v>
       </c>
       <c r="G571" t="n">
         <v>4987112</v>
@@ -13626,7 +13626,7 @@
         <v>2509.12841796875</v>
       </c>
       <c r="F573" t="n">
-        <v>2483.7353515625</v>
+        <v>2483.735107421875</v>
       </c>
       <c r="G573" t="n">
         <v>12536120</v>
@@ -13718,7 +13718,7 @@
         <v>2561.924072265625</v>
       </c>
       <c r="F577" t="n">
-        <v>2535.996337890625</v>
+        <v>2535.99658203125</v>
       </c>
       <c r="G577" t="n">
         <v>6113833</v>
@@ -13810,7 +13810,7 @@
         <v>2566.3544921875</v>
       </c>
       <c r="F581" t="n">
-        <v>2540.38232421875</v>
+        <v>2540.382080078125</v>
       </c>
       <c r="G581" t="n">
         <v>4733503</v>
@@ -13833,7 +13833,7 @@
         <v>2486.238037109375</v>
       </c>
       <c r="F582" t="n">
-        <v>2461.07666015625</v>
+        <v>2461.076416015625</v>
       </c>
       <c r="G582" t="n">
         <v>9623830</v>
@@ -13948,7 +13948,7 @@
         <v>2260.703125</v>
       </c>
       <c r="F587" t="n">
-        <v>2237.82421875</v>
+        <v>2237.823974609375</v>
       </c>
       <c r="G587" t="n">
         <v>8321949</v>
@@ -13971,7 +13971,7 @@
         <v>2214.6455078125</v>
       </c>
       <c r="F588" t="n">
-        <v>2192.232421875</v>
+        <v>2192.232666015625</v>
       </c>
       <c r="G588" t="n">
         <v>10245160</v>
@@ -14017,7 +14017,7 @@
         <v>2240.304931640625</v>
       </c>
       <c r="F590" t="n">
-        <v>2217.63232421875</v>
+        <v>2217.632080078125</v>
       </c>
       <c r="G590" t="n">
         <v>6718955</v>
@@ -14040,7 +14040,7 @@
         <v>2334.404541015625</v>
       </c>
       <c r="F591" t="n">
-        <v>2310.779296875</v>
+        <v>2310.779541015625</v>
       </c>
       <c r="G591" t="n">
         <v>8275914</v>
@@ -14178,7 +14178,7 @@
         <v>2410.875244140625</v>
       </c>
       <c r="F597" t="n">
-        <v>2386.4765625</v>
+        <v>2386.476318359375</v>
       </c>
       <c r="G597" t="n">
         <v>6357272</v>
@@ -14201,7 +14201,7 @@
         <v>2387.892578125</v>
       </c>
       <c r="F598" t="n">
-        <v>2363.726318359375</v>
+        <v>2363.72607421875</v>
       </c>
       <c r="G598" t="n">
         <v>8941011</v>
@@ -14293,7 +14293,7 @@
         <v>2430.7197265625</v>
       </c>
       <c r="F602" t="n">
-        <v>2406.1201171875</v>
+        <v>2406.119873046875</v>
       </c>
       <c r="G602" t="n">
         <v>4888494</v>
@@ -14316,7 +14316,7 @@
         <v>2514.528076171875</v>
       </c>
       <c r="F603" t="n">
-        <v>2489.080078125</v>
+        <v>2489.080322265625</v>
       </c>
       <c r="G603" t="n">
         <v>11063284</v>
@@ -14385,7 +14385,7 @@
         <v>2559.247314453125</v>
       </c>
       <c r="F606" t="n">
-        <v>2533.346923828125</v>
+        <v>2533.3466796875</v>
       </c>
       <c r="G606" t="n">
         <v>6179127</v>
@@ -14477,7 +14477,7 @@
         <v>2457.855712890625</v>
       </c>
       <c r="F610" t="n">
-        <v>2432.9814453125</v>
+        <v>2432.981201171875</v>
       </c>
       <c r="G610" t="n">
         <v>8810401</v>
@@ -14546,7 +14546,7 @@
         <v>2362.879150390625</v>
       </c>
       <c r="F613" t="n">
-        <v>2338.9658203125</v>
+        <v>2338.966064453125</v>
       </c>
       <c r="G613" t="n">
         <v>8555737</v>
@@ -14592,7 +14592,7 @@
         <v>2347.234375</v>
       </c>
       <c r="F615" t="n">
-        <v>2323.4794921875</v>
+        <v>2323.479736328125</v>
       </c>
       <c r="G615" t="n">
         <v>6033398</v>
@@ -14684,7 +14684,7 @@
         <v>2307.54541015625</v>
       </c>
       <c r="F619" t="n">
-        <v>2284.192138671875</v>
+        <v>2284.1923828125</v>
       </c>
       <c r="G619" t="n">
         <v>7120117</v>
@@ -14707,7 +14707,7 @@
         <v>2300.715087890625</v>
       </c>
       <c r="F620" t="n">
-        <v>2277.43115234375</v>
+        <v>2277.430908203125</v>
       </c>
       <c r="G620" t="n">
         <v>7737264</v>
@@ -14914,7 +14914,7 @@
         <v>2207.261474609375</v>
       </c>
       <c r="F629" t="n">
-        <v>2184.923095703125</v>
+        <v>2184.92333984375</v>
       </c>
       <c r="G629" t="n">
         <v>9505054</v>
@@ -14937,7 +14937,7 @@
         <v>2237.259033203125</v>
       </c>
       <c r="F630" t="n">
-        <v>2214.616943359375</v>
+        <v>2214.6171875</v>
       </c>
       <c r="G630" t="n">
         <v>6923733</v>
@@ -14960,7 +14960,7 @@
         <v>2234.074462890625</v>
       </c>
       <c r="F631" t="n">
-        <v>2211.464599609375</v>
+        <v>2211.46484375</v>
       </c>
       <c r="G631" t="n">
         <v>5389494</v>
@@ -14983,7 +14983,7 @@
         <v>2194.477783203125</v>
       </c>
       <c r="F632" t="n">
-        <v>2172.268798828125</v>
+        <v>2172.26904296875</v>
       </c>
       <c r="G632" t="n">
         <v>7112066</v>
@@ -15006,7 +15006,7 @@
         <v>2212.568603515625</v>
       </c>
       <c r="F633" t="n">
-        <v>2190.176513671875</v>
+        <v>2190.1767578125</v>
       </c>
       <c r="G633" t="n">
         <v>8485157</v>
@@ -15029,7 +15029,7 @@
         <v>2216.860595703125</v>
       </c>
       <c r="F634" t="n">
-        <v>2194.425048828125</v>
+        <v>2194.42529296875</v>
       </c>
       <c r="G634" t="n">
         <v>4801605</v>
@@ -15052,7 +15052,7 @@
         <v>2235.736083984375</v>
       </c>
       <c r="F635" t="n">
-        <v>2213.109375</v>
+        <v>2213.109619140625</v>
       </c>
       <c r="G635" t="n">
         <v>7580454</v>
@@ -15213,7 +15213,7 @@
         <v>2232.9208984375</v>
       </c>
       <c r="F642" t="n">
-        <v>2210.322998046875</v>
+        <v>2210.32275390625</v>
       </c>
       <c r="G642" t="n">
         <v>4327543</v>
@@ -15259,7 +15259,7 @@
         <v>2316.221435546875</v>
       </c>
       <c r="F644" t="n">
-        <v>2292.780517578125</v>
+        <v>2292.7802734375</v>
       </c>
       <c r="G644" t="n">
         <v>7565341</v>
@@ -15305,7 +15305,7 @@
         <v>2385.631103515625</v>
       </c>
       <c r="F646" t="n">
-        <v>2361.487548828125</v>
+        <v>2361.48779296875</v>
       </c>
       <c r="G646" t="n">
         <v>6958956</v>
@@ -15420,7 +15420,7 @@
         <v>2383.646728515625</v>
       </c>
       <c r="F651" t="n">
-        <v>2359.5234375</v>
+        <v>2359.523193359375</v>
       </c>
       <c r="G651" t="n">
         <v>5362344</v>
@@ -15466,7 +15466,7 @@
         <v>2430.258056640625</v>
       </c>
       <c r="F653" t="n">
-        <v>2405.662841796875</v>
+        <v>2405.6630859375</v>
       </c>
       <c r="G653" t="n">
         <v>6325293</v>
@@ -27233,111 +27233,19 @@
         <v>2914</v>
       </c>
       <c r="C1165" t="n">
-        <v>2972</v>
+        <v>2949.89990234375</v>
       </c>
       <c r="D1165" t="n">
         <v>2891.75</v>
       </c>
       <c r="E1165" t="n">
-        <v>2959.60009765625</v>
+        <v>2947</v>
       </c>
       <c r="F1165" t="n">
-        <v>2959.60009765625</v>
+        <v>2947</v>
       </c>
       <c r="G1165" t="n">
-        <v>11174688</v>
-      </c>
-    </row>
-    <row r="1166">
-      <c r="A1166" s="2" t="n">
-        <v>45548</v>
-      </c>
-      <c r="B1166" t="n">
-        <v>2952.800048828125</v>
-      </c>
-      <c r="C1166" t="n">
-        <v>2966.300048828125</v>
-      </c>
-      <c r="D1166" t="n">
-        <v>2939</v>
-      </c>
-      <c r="E1166" t="n">
-        <v>2945.25</v>
-      </c>
-      <c r="F1166" t="n">
-        <v>2945.25</v>
-      </c>
-      <c r="G1166" t="n">
-        <v>4355664</v>
-      </c>
-    </row>
-    <row r="1167">
-      <c r="A1167" s="2" t="n">
-        <v>45551</v>
-      </c>
-      <c r="B1167" t="n">
-        <v>2955.10009765625</v>
-      </c>
-      <c r="C1167" t="n">
-        <v>2961.800048828125</v>
-      </c>
-      <c r="D1167" t="n">
-        <v>2929.5</v>
-      </c>
-      <c r="E1167" t="n">
-        <v>2942.699951171875</v>
-      </c>
-      <c r="F1167" t="n">
-        <v>2942.699951171875</v>
-      </c>
-      <c r="G1167" t="n">
-        <v>2740887</v>
-      </c>
-    </row>
-    <row r="1168">
-      <c r="A1168" s="2" t="n">
-        <v>45552</v>
-      </c>
-      <c r="B1168" t="n">
-        <v>2948</v>
-      </c>
-      <c r="C1168" t="n">
-        <v>2954.949951171875</v>
-      </c>
-      <c r="D1168" t="n">
-        <v>2933.25</v>
-      </c>
-      <c r="E1168" t="n">
-        <v>2944.60009765625</v>
-      </c>
-      <c r="F1168" t="n">
-        <v>2944.60009765625</v>
-      </c>
-      <c r="G1168" t="n">
-        <v>2967664</v>
-      </c>
-    </row>
-    <row r="1169">
-      <c r="A1169" s="2" t="n">
-        <v>45553</v>
-      </c>
-      <c r="B1169" t="n">
-        <v>2940</v>
-      </c>
-      <c r="C1169" t="n">
-        <v>2951</v>
-      </c>
-      <c r="D1169" t="n">
-        <v>2937.5</v>
-      </c>
-      <c r="E1169" t="n">
-        <v>2949.050048828125</v>
-      </c>
-      <c r="F1169" t="n">
-        <v>2949.050048828125</v>
-      </c>
-      <c r="G1169" t="n">
-        <v>274791</v>
+        <v>6610010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>